<commit_message>
corrected section heading labeling error
</commit_message>
<xml_diff>
--- a/distribution/reference_documents/working_material/AVCDL mappings.xlsx
+++ b/distribution/reference_documents/working_material/AVCDL mappings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charleswilson/Documents/projects/AVCDL/source/reference_documents/working_material/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charleswilson/Documents/projects/AVCDL/distribution/reference_documents/working_material/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F3BCE2-A3AE-5743-A786-C2A3D6E3EA55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F19A13D-BE3D-3D44-9705-0CDF04C3ECD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15100" yWindow="3160" windowWidth="32160" windowHeight="23180" activeTab="4" xr2:uid="{3326EDE7-94E3-604E-AF7C-9D9EC9C448CE}"/>
+    <workbookView xWindow="31260" yWindow="2720" windowWidth="32160" windowHeight="23180" xr2:uid="{3326EDE7-94E3-604E-AF7C-9D9EC9C448CE}"/>
   </bookViews>
   <sheets>
     <sheet name="ISO 21434 work products" sheetId="1" r:id="rId1"/>
@@ -2286,7 +2286,7 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="252">
+  <cellXfs count="253">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2710,7 +2710,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -2731,6 +2731,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
@@ -3516,8 +3519,12 @@
   </sheetPr>
   <dimension ref="A1:AA63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="20320" ySplit="760" topLeftCell="H12" activePane="bottomRight"/>
+      <selection activeCell="C1" sqref="C1:D1"/>
+      <selection pane="topRight" activeCell="H1" sqref="H1:X1"/>
+      <selection pane="bottomLeft" activeCell="B48" sqref="B48:G48"/>
+      <selection pane="bottomRight" activeCell="P61" sqref="P61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4689,7 +4696,7 @@
     <row r="48" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A48" s="85"/>
       <c r="B48" s="144" t="s">
-        <v>30</v>
+        <v>550</v>
       </c>
       <c r="C48" s="144"/>
       <c r="D48" s="144"/>
@@ -4975,7 +4982,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC060107-2EBE-164D-8193-C4628FFE16DF}">
   <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
@@ -4998,11 +5005,11 @@
       <c r="B1" s="159" t="s">
         <v>302</v>
       </c>
-      <c r="C1" s="152"/>
-      <c r="D1" s="160" t="s">
+      <c r="C1" s="160"/>
+      <c r="D1" s="161" t="s">
         <v>303</v>
       </c>
-      <c r="E1" s="161"/>
+      <c r="E1" s="162"/>
       <c r="F1" s="158" t="s">
         <v>308</v>
       </c>
@@ -5221,16 +5228,16 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="145"/>
-      <c r="B11" s="164" t="s">
+      <c r="B11" s="165" t="s">
         <v>270</v>
       </c>
-      <c r="C11" s="163" t="s">
+      <c r="C11" s="164" t="s">
         <v>274</v>
       </c>
-      <c r="D11" s="163" t="s">
+      <c r="D11" s="164" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="163" t="s">
+      <c r="E11" s="164" t="s">
         <v>10</v>
       </c>
       <c r="F11" s="75" t="s">
@@ -5248,10 +5255,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="145"/>
-      <c r="B12" s="164"/>
-      <c r="C12" s="163"/>
-      <c r="D12" s="163"/>
-      <c r="E12" s="163"/>
+      <c r="B12" s="165"/>
+      <c r="C12" s="164"/>
+      <c r="D12" s="164"/>
+      <c r="E12" s="164"/>
       <c r="F12" s="75" t="s">
         <v>375</v>
       </c>
@@ -5404,7 +5411,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="145"/>
-      <c r="B18" s="162" t="s">
+      <c r="B18" s="163" t="s">
         <v>291</v>
       </c>
       <c r="C18" s="155" t="s">
@@ -5431,7 +5438,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="145"/>
-      <c r="B19" s="162"/>
+      <c r="B19" s="163"/>
       <c r="C19" s="155"/>
       <c r="D19" s="155"/>
       <c r="E19" s="155"/>
@@ -5450,7 +5457,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="145"/>
-      <c r="B20" s="162"/>
+      <c r="B20" s="163"/>
       <c r="C20" s="155"/>
       <c r="D20" s="155"/>
       <c r="E20" s="155"/>
@@ -6427,22 +6434,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="E1" s="167" t="s">
+      <c r="E1" s="168" t="s">
         <v>527</v>
       </c>
-      <c r="F1" s="167"/>
-      <c r="G1" s="167"/>
-      <c r="H1" s="167"/>
-      <c r="I1" s="167"/>
-      <c r="J1" s="167"/>
-      <c r="K1" s="167"/>
-      <c r="L1" s="167"/>
-      <c r="M1" s="167"/>
-      <c r="N1" s="167"/>
-      <c r="O1" s="167"/>
-      <c r="P1" s="167"/>
-      <c r="Q1" s="167"/>
-      <c r="R1" s="167"/>
+      <c r="F1" s="168"/>
+      <c r="G1" s="168"/>
+      <c r="H1" s="168"/>
+      <c r="I1" s="168"/>
+      <c r="J1" s="168"/>
+      <c r="K1" s="168"/>
+      <c r="L1" s="168"/>
+      <c r="M1" s="168"/>
+      <c r="N1" s="168"/>
+      <c r="O1" s="168"/>
+      <c r="P1" s="168"/>
+      <c r="Q1" s="168"/>
+      <c r="R1" s="168"/>
       <c r="S1" s="10"/>
     </row>
     <row r="2" spans="1:19" s="48" customFormat="1" ht="55" x14ac:dyDescent="0.2">
@@ -6494,10 +6501,10 @@
       <c r="S2" s="10"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A3" s="187" t="s">
+      <c r="A3" s="188" t="s">
         <v>613</v>
       </c>
-      <c r="B3" s="176" t="s">
+      <c r="B3" s="177" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="31" t="s">
@@ -6525,8 +6532,8 @@
       <c r="S3" s="10"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A4" s="188"/>
-      <c r="B4" s="177"/>
+      <c r="A4" s="189"/>
+      <c r="B4" s="178"/>
       <c r="C4" s="31" t="s">
         <v>155</v>
       </c>
@@ -6552,8 +6559,8 @@
       <c r="S4" s="10"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A5" s="188"/>
-      <c r="B5" s="177"/>
+      <c r="A5" s="189"/>
+      <c r="B5" s="178"/>
       <c r="C5" s="31" t="s">
         <v>156</v>
       </c>
@@ -6579,8 +6586,8 @@
       <c r="S5" s="10"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" s="188"/>
-      <c r="B6" s="177"/>
+      <c r="A6" s="189"/>
+      <c r="B6" s="178"/>
       <c r="C6" s="30" t="s">
         <v>157</v>
       </c>
@@ -6604,8 +6611,8 @@
       <c r="S6" s="10"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A7" s="188"/>
-      <c r="B7" s="177"/>
+      <c r="A7" s="189"/>
+      <c r="B7" s="178"/>
       <c r="C7" s="30" t="s">
         <v>158</v>
       </c>
@@ -6629,8 +6636,8 @@
       <c r="S7" s="10"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8" s="188"/>
-      <c r="B8" s="177"/>
+      <c r="A8" s="189"/>
+      <c r="B8" s="178"/>
       <c r="C8" s="31" t="s">
         <v>159</v>
       </c>
@@ -6656,8 +6663,8 @@
       <c r="S8" s="10"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A9" s="188"/>
-      <c r="B9" s="177"/>
+      <c r="A9" s="189"/>
+      <c r="B9" s="178"/>
       <c r="C9" s="31" t="s">
         <v>161</v>
       </c>
@@ -6683,8 +6690,8 @@
       <c r="S9" s="10"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A10" s="188"/>
-      <c r="B10" s="177"/>
+      <c r="A10" s="189"/>
+      <c r="B10" s="178"/>
       <c r="C10" s="31" t="s">
         <v>162</v>
       </c>
@@ -6710,8 +6717,8 @@
       <c r="S10" s="10"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A11" s="188"/>
-      <c r="B11" s="177"/>
+      <c r="A11" s="189"/>
+      <c r="B11" s="178"/>
       <c r="C11" s="30" t="s">
         <v>163</v>
       </c>
@@ -6735,8 +6742,8 @@
       <c r="S11" s="10"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A12" s="188"/>
-      <c r="B12" s="173" t="s">
+      <c r="A12" s="189"/>
+      <c r="B12" s="174" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="31" t="s">
@@ -6764,8 +6771,8 @@
       <c r="S12" s="10"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A13" s="188"/>
-      <c r="B13" s="174"/>
+      <c r="A13" s="189"/>
+      <c r="B13" s="175"/>
       <c r="C13" s="31" t="s">
         <v>162</v>
       </c>
@@ -6791,8 +6798,8 @@
       <c r="S13" s="10"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A14" s="188"/>
-      <c r="B14" s="179" t="s">
+      <c r="A14" s="189"/>
+      <c r="B14" s="180" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="23" t="s">
@@ -6820,8 +6827,8 @@
       <c r="S14" s="10"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A15" s="188"/>
-      <c r="B15" s="179"/>
+      <c r="A15" s="189"/>
+      <c r="B15" s="180"/>
       <c r="C15" s="22" t="s">
         <v>160</v>
       </c>
@@ -6845,7 +6852,7 @@
       <c r="S15" s="10"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" s="188"/>
+      <c r="A16" s="189"/>
       <c r="B16" s="125" t="s">
         <v>6</v>
       </c>
@@ -6872,7 +6879,7 @@
       <c r="S16" s="10"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A17" s="189"/>
+      <c r="A17" s="190"/>
       <c r="B17" s="22" t="s">
         <v>7</v>
       </c>
@@ -6899,10 +6906,10 @@
       <c r="S17" s="10"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A18" s="187" t="s">
+      <c r="A18" s="188" t="s">
         <v>612</v>
       </c>
-      <c r="B18" s="176" t="s">
+      <c r="B18" s="177" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="30" t="s">
@@ -6928,8 +6935,8 @@
       <c r="S18" s="10"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A19" s="188"/>
-      <c r="B19" s="177"/>
+      <c r="A19" s="189"/>
+      <c r="B19" s="178"/>
       <c r="C19" s="30" t="s">
         <v>167</v>
       </c>
@@ -6953,8 +6960,8 @@
       <c r="S19" s="10"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A20" s="188"/>
-      <c r="B20" s="177"/>
+      <c r="A20" s="189"/>
+      <c r="B20" s="178"/>
       <c r="C20" s="30" t="s">
         <v>168</v>
       </c>
@@ -6978,8 +6985,8 @@
       <c r="S20" s="10"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A21" s="188"/>
-      <c r="B21" s="177"/>
+      <c r="A21" s="189"/>
+      <c r="B21" s="178"/>
       <c r="C21" s="30" t="s">
         <v>169</v>
       </c>
@@ -7003,8 +7010,8 @@
       <c r="S21" s="10"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A22" s="188"/>
-      <c r="B22" s="177"/>
+      <c r="A22" s="189"/>
+      <c r="B22" s="178"/>
       <c r="C22" s="30" t="s">
         <v>170</v>
       </c>
@@ -7028,8 +7035,8 @@
       <c r="S22" s="10"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A23" s="188"/>
-      <c r="B23" s="177"/>
+      <c r="A23" s="189"/>
+      <c r="B23" s="178"/>
       <c r="C23" s="30" t="s">
         <v>171</v>
       </c>
@@ -7053,8 +7060,8 @@
       <c r="S23" s="10"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A24" s="188"/>
-      <c r="B24" s="177"/>
+      <c r="A24" s="189"/>
+      <c r="B24" s="178"/>
       <c r="C24" s="30" t="s">
         <v>172</v>
       </c>
@@ -7078,8 +7085,8 @@
       <c r="S24" s="10"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A25" s="188"/>
-      <c r="B25" s="177"/>
+      <c r="A25" s="189"/>
+      <c r="B25" s="178"/>
       <c r="C25" s="31" t="s">
         <v>173</v>
       </c>
@@ -7105,8 +7112,8 @@
       <c r="S25" s="10"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A26" s="188"/>
-      <c r="B26" s="177"/>
+      <c r="A26" s="189"/>
+      <c r="B26" s="178"/>
       <c r="C26" s="31" t="s">
         <v>174</v>
       </c>
@@ -7132,8 +7139,8 @@
       <c r="S26" s="10"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A27" s="188"/>
-      <c r="B27" s="177"/>
+      <c r="A27" s="189"/>
+      <c r="B27" s="178"/>
       <c r="C27" s="30" t="s">
         <v>175</v>
       </c>
@@ -7157,8 +7164,8 @@
       <c r="S27" s="10"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A28" s="188"/>
-      <c r="B28" s="177"/>
+      <c r="A28" s="189"/>
+      <c r="B28" s="178"/>
       <c r="C28" s="30" t="s">
         <v>176</v>
       </c>
@@ -7182,8 +7189,8 @@
       <c r="S28" s="10"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A29" s="188"/>
-      <c r="B29" s="177"/>
+      <c r="A29" s="189"/>
+      <c r="B29" s="178"/>
       <c r="C29" s="30" t="s">
         <v>177</v>
       </c>
@@ -7207,8 +7214,8 @@
       <c r="S29" s="10"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A30" s="188"/>
-      <c r="B30" s="177"/>
+      <c r="A30" s="189"/>
+      <c r="B30" s="178"/>
       <c r="C30" s="30" t="s">
         <v>178</v>
       </c>
@@ -7232,8 +7239,8 @@
       <c r="S30" s="10"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A31" s="188"/>
-      <c r="B31" s="177"/>
+      <c r="A31" s="189"/>
+      <c r="B31" s="178"/>
       <c r="C31" s="30" t="s">
         <v>179</v>
       </c>
@@ -7257,8 +7264,8 @@
       <c r="S31" s="10"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A32" s="188"/>
-      <c r="B32" s="177"/>
+      <c r="A32" s="189"/>
+      <c r="B32" s="178"/>
       <c r="C32" s="30" t="s">
         <v>180</v>
       </c>
@@ -7282,8 +7289,8 @@
       <c r="S32" s="10"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A33" s="188"/>
-      <c r="B33" s="177"/>
+      <c r="A33" s="189"/>
+      <c r="B33" s="178"/>
       <c r="C33" s="30" t="s">
         <v>181</v>
       </c>
@@ -7307,8 +7314,8 @@
       <c r="S33" s="10"/>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A34" s="188"/>
-      <c r="B34" s="177"/>
+      <c r="A34" s="189"/>
+      <c r="B34" s="178"/>
       <c r="C34" s="30" t="s">
         <v>182</v>
       </c>
@@ -7332,8 +7339,8 @@
       <c r="S34" s="10"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A35" s="188"/>
-      <c r="B35" s="177"/>
+      <c r="A35" s="189"/>
+      <c r="B35" s="178"/>
       <c r="C35" s="30" t="s">
         <v>183</v>
       </c>
@@ -7357,8 +7364,8 @@
       <c r="S35" s="10"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A36" s="188"/>
-      <c r="B36" s="177"/>
+      <c r="A36" s="189"/>
+      <c r="B36" s="178"/>
       <c r="C36" s="30" t="s">
         <v>184</v>
       </c>
@@ -7382,8 +7389,8 @@
       <c r="S36" s="10"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A37" s="188"/>
-      <c r="B37" s="180"/>
+      <c r="A37" s="189"/>
+      <c r="B37" s="181"/>
       <c r="C37" s="30" t="s">
         <v>185</v>
       </c>
@@ -7407,7 +7414,7 @@
       <c r="S37" s="10"/>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A38" s="188"/>
+      <c r="A38" s="189"/>
       <c r="B38" s="22" t="s">
         <v>15</v>
       </c>
@@ -7434,8 +7441,8 @@
       <c r="S38" s="10"/>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A39" s="188"/>
-      <c r="B39" s="168" t="s">
+      <c r="A39" s="189"/>
+      <c r="B39" s="169" t="s">
         <v>16</v>
       </c>
       <c r="C39" s="30" t="s">
@@ -7461,8 +7468,8 @@
       <c r="S39" s="10"/>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A40" s="188"/>
-      <c r="B40" s="181"/>
+      <c r="A40" s="189"/>
+      <c r="B40" s="182"/>
       <c r="C40" s="30" t="s">
         <v>188</v>
       </c>
@@ -7486,8 +7493,8 @@
       <c r="S40" s="10"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A41" s="188"/>
-      <c r="B41" s="181"/>
+      <c r="A41" s="189"/>
+      <c r="B41" s="182"/>
       <c r="C41" s="30" t="s">
         <v>189</v>
       </c>
@@ -7511,8 +7518,8 @@
       <c r="S41" s="10"/>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A42" s="188"/>
-      <c r="B42" s="181"/>
+      <c r="A42" s="189"/>
+      <c r="B42" s="182"/>
       <c r="C42" s="30" t="s">
         <v>190</v>
       </c>
@@ -7536,8 +7543,8 @@
       <c r="S42" s="10"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A43" s="188"/>
-      <c r="B43" s="181"/>
+      <c r="A43" s="189"/>
+      <c r="B43" s="182"/>
       <c r="C43" s="30" t="s">
         <v>191</v>
       </c>
@@ -7561,8 +7568,8 @@
       <c r="S43" s="10"/>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A44" s="188"/>
-      <c r="B44" s="181"/>
+      <c r="A44" s="189"/>
+      <c r="B44" s="182"/>
       <c r="C44" s="30" t="s">
         <v>581</v>
       </c>
@@ -7586,8 +7593,8 @@
       <c r="S44" s="10"/>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A45" s="188"/>
-      <c r="B45" s="181"/>
+      <c r="A45" s="189"/>
+      <c r="B45" s="182"/>
       <c r="C45" s="30" t="s">
         <v>552</v>
       </c>
@@ -7611,8 +7618,8 @@
       <c r="S45" s="10"/>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A46" s="188"/>
-      <c r="B46" s="169"/>
+      <c r="A46" s="189"/>
+      <c r="B46" s="170"/>
       <c r="C46" s="30" t="s">
         <v>553</v>
       </c>
@@ -7636,8 +7643,8 @@
       <c r="S46" s="10"/>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A47" s="188"/>
-      <c r="B47" s="168" t="s">
+      <c r="A47" s="189"/>
+      <c r="B47" s="169" t="s">
         <v>17</v>
       </c>
       <c r="C47" s="30" t="s">
@@ -7663,8 +7670,8 @@
       <c r="S47" s="10"/>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A48" s="189"/>
-      <c r="B48" s="169"/>
+      <c r="A48" s="190"/>
+      <c r="B48" s="170"/>
       <c r="C48" s="30" t="s">
         <v>555</v>
       </c>
@@ -7709,10 +7716,10 @@
       <c r="S49" s="10"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A50" s="184" t="s">
+      <c r="A50" s="185" t="s">
         <v>619</v>
       </c>
-      <c r="B50" s="168" t="s">
+      <c r="B50" s="169" t="s">
         <v>262</v>
       </c>
       <c r="C50" s="30" t="s">
@@ -7738,8 +7745,8 @@
       <c r="S50" s="10"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A51" s="185"/>
-      <c r="B51" s="169"/>
+      <c r="A51" s="186"/>
+      <c r="B51" s="170"/>
       <c r="C51" s="30" t="s">
         <v>126</v>
       </c>
@@ -7763,7 +7770,7 @@
       <c r="S51" s="10"/>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A52" s="185"/>
+      <c r="A52" s="186"/>
       <c r="B52" s="22" t="s">
         <v>263</v>
       </c>
@@ -7790,8 +7797,8 @@
       <c r="S52" s="10"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A53" s="185"/>
-      <c r="B53" s="176" t="s">
+      <c r="A53" s="186"/>
+      <c r="B53" s="177" t="s">
         <v>23</v>
       </c>
       <c r="C53" s="31" t="s">
@@ -7819,8 +7826,8 @@
       <c r="S53" s="10"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A54" s="185"/>
-      <c r="B54" s="177"/>
+      <c r="A54" s="186"/>
+      <c r="B54" s="178"/>
       <c r="C54" s="31" t="s">
         <v>251</v>
       </c>
@@ -7846,8 +7853,8 @@
       <c r="S54" s="10"/>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A55" s="186"/>
-      <c r="B55" s="177"/>
+      <c r="A55" s="187"/>
+      <c r="B55" s="178"/>
       <c r="C55" s="30" t="s">
         <v>252</v>
       </c>
@@ -7892,7 +7899,7 @@
       <c r="S56" s="10"/>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A57" s="184" t="s">
+      <c r="A57" s="185" t="s">
         <v>614</v>
       </c>
       <c r="B57" s="23" t="s">
@@ -7923,7 +7930,7 @@
       <c r="S57" s="10"/>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A58" s="185"/>
+      <c r="A58" s="186"/>
       <c r="B58" s="23" t="s">
         <v>43</v>
       </c>
@@ -7952,7 +7959,7 @@
       <c r="S58" s="10"/>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A59" s="185"/>
+      <c r="A59" s="186"/>
       <c r="B59" s="23" t="s">
         <v>44</v>
       </c>
@@ -7983,7 +7990,7 @@
       <c r="S59" s="10"/>
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A60" s="185"/>
+      <c r="A60" s="186"/>
       <c r="B60" s="23" t="s">
         <v>45</v>
       </c>
@@ -8012,8 +8019,8 @@
       <c r="S60" s="10"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A61" s="185"/>
-      <c r="B61" s="173" t="s">
+      <c r="A61" s="186"/>
+      <c r="B61" s="174" t="s">
         <v>46</v>
       </c>
       <c r="C61" s="31" t="s">
@@ -8043,8 +8050,8 @@
       <c r="S61" s="10"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A62" s="185"/>
-      <c r="B62" s="174"/>
+      <c r="A62" s="186"/>
+      <c r="B62" s="175"/>
       <c r="C62" s="31" t="s">
         <v>140</v>
       </c>
@@ -8072,7 +8079,7 @@
       <c r="S62" s="10"/>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A63" s="185"/>
+      <c r="A63" s="186"/>
       <c r="B63" s="23" t="s">
         <v>47</v>
       </c>
@@ -8101,7 +8108,7 @@
       <c r="S63" s="10"/>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A64" s="186"/>
+      <c r="A64" s="187"/>
       <c r="B64" s="22" t="s">
         <v>539</v>
       </c>
@@ -8149,10 +8156,10 @@
       <c r="S65" s="10"/>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A66" s="184" t="s">
+      <c r="A66" s="185" t="s">
         <v>605</v>
       </c>
-      <c r="B66" s="175" t="s">
+      <c r="B66" s="176" t="s">
         <v>55</v>
       </c>
       <c r="C66" s="30" t="s">
@@ -8178,8 +8185,8 @@
       <c r="S66" s="10"/>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A67" s="185"/>
-      <c r="B67" s="175"/>
+      <c r="A67" s="186"/>
+      <c r="B67" s="176"/>
       <c r="C67" s="30" t="s">
         <v>256</v>
       </c>
@@ -8203,8 +8210,8 @@
       <c r="S67" s="10"/>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A68" s="185"/>
-      <c r="B68" s="168" t="s">
+      <c r="A68" s="186"/>
+      <c r="B68" s="169" t="s">
         <v>56</v>
       </c>
       <c r="C68" s="30" t="s">
@@ -8230,8 +8237,8 @@
       <c r="S68" s="10"/>
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A69" s="185"/>
-      <c r="B69" s="169"/>
+      <c r="A69" s="186"/>
+      <c r="B69" s="170"/>
       <c r="C69" s="30" t="s">
         <v>117</v>
       </c>
@@ -8255,7 +8262,7 @@
       <c r="S69" s="10"/>
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A70" s="185"/>
+      <c r="A70" s="186"/>
       <c r="B70" s="23" t="s">
         <v>57</v>
       </c>
@@ -8284,7 +8291,7 @@
       <c r="S70" s="10"/>
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A71" s="185"/>
+      <c r="A71" s="186"/>
       <c r="B71" s="23" t="s">
         <v>58</v>
       </c>
@@ -8313,7 +8320,7 @@
       <c r="S71" s="10"/>
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A72" s="185"/>
+      <c r="A72" s="186"/>
       <c r="B72" s="23" t="s">
         <v>59</v>
       </c>
@@ -8342,8 +8349,8 @@
       <c r="S72" s="10"/>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A73" s="185"/>
-      <c r="B73" s="170" t="s">
+      <c r="A73" s="186"/>
+      <c r="B73" s="171" t="s">
         <v>60</v>
       </c>
       <c r="C73" s="31" t="s">
@@ -8371,8 +8378,8 @@
       <c r="S73" s="10"/>
     </row>
     <row r="74" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A74" s="185"/>
-      <c r="B74" s="171"/>
+      <c r="A74" s="186"/>
+      <c r="B74" s="172"/>
       <c r="C74" s="30" t="s">
         <v>122</v>
       </c>
@@ -8396,8 +8403,8 @@
       <c r="S74" s="10"/>
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A75" s="185"/>
-      <c r="B75" s="172"/>
+      <c r="A75" s="186"/>
+      <c r="B75" s="173"/>
       <c r="C75" s="30" t="s">
         <v>123</v>
       </c>
@@ -8421,7 +8428,7 @@
       <c r="S75" s="10"/>
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A76" s="186"/>
+      <c r="A76" s="187"/>
       <c r="B76" s="22" t="s">
         <v>61</v>
       </c>
@@ -8448,10 +8455,10 @@
       <c r="S76" s="10"/>
     </row>
     <row r="77" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A77" s="184" t="s">
+      <c r="A77" s="185" t="s">
         <v>615</v>
       </c>
-      <c r="B77" s="170" t="s">
+      <c r="B77" s="171" t="s">
         <v>75</v>
       </c>
       <c r="C77" s="31" t="s">
@@ -8479,8 +8486,8 @@
       <c r="S77" s="10"/>
     </row>
     <row r="78" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A78" s="185"/>
-      <c r="B78" s="171"/>
+      <c r="A78" s="186"/>
+      <c r="B78" s="172"/>
       <c r="C78" s="30" t="s">
         <v>144</v>
       </c>
@@ -8504,7 +8511,7 @@
       <c r="S78" s="10"/>
     </row>
     <row r="79" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A79" s="185"/>
+      <c r="A79" s="186"/>
       <c r="B79" s="124" t="s">
         <v>76</v>
       </c>
@@ -8531,8 +8538,8 @@
       <c r="S79" s="10"/>
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A80" s="185"/>
-      <c r="B80" s="175" t="s">
+      <c r="A80" s="186"/>
+      <c r="B80" s="176" t="s">
         <v>77</v>
       </c>
       <c r="C80" s="30" t="s">
@@ -8558,8 +8565,8 @@
       <c r="S80" s="10"/>
     </row>
     <row r="81" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A81" s="185"/>
-      <c r="B81" s="175"/>
+      <c r="A81" s="186"/>
+      <c r="B81" s="176"/>
       <c r="C81" s="30" t="s">
         <v>147</v>
       </c>
@@ -8583,7 +8590,7 @@
       <c r="S81" s="10"/>
     </row>
     <row r="82" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A82" s="185"/>
+      <c r="A82" s="186"/>
       <c r="B82" s="124" t="s">
         <v>78</v>
       </c>
@@ -8610,8 +8617,8 @@
       <c r="S82" s="10"/>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A83" s="185"/>
-      <c r="B83" s="175" t="s">
+      <c r="A83" s="186"/>
+      <c r="B83" s="176" t="s">
         <v>79</v>
       </c>
       <c r="C83" s="30" t="s">
@@ -8637,8 +8644,8 @@
       <c r="S83" s="10"/>
     </row>
     <row r="84" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A84" s="185"/>
-      <c r="B84" s="175"/>
+      <c r="A84" s="186"/>
+      <c r="B84" s="176"/>
       <c r="C84" s="30" t="s">
         <v>560</v>
       </c>
@@ -8662,8 +8669,8 @@
       <c r="S84" s="10"/>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A85" s="185"/>
-      <c r="B85" s="175"/>
+      <c r="A85" s="186"/>
+      <c r="B85" s="176"/>
       <c r="C85" s="30" t="s">
         <v>152</v>
       </c>
@@ -8687,7 +8694,7 @@
       <c r="S85" s="10"/>
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A86" s="185"/>
+      <c r="A86" s="186"/>
       <c r="B86" s="125" t="s">
         <v>80</v>
       </c>
@@ -8714,8 +8721,8 @@
       <c r="S86" s="10"/>
     </row>
     <row r="87" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A87" s="185"/>
-      <c r="B87" s="175" t="s">
+      <c r="A87" s="186"/>
+      <c r="B87" s="176" t="s">
         <v>81</v>
       </c>
       <c r="C87" s="30" t="s">
@@ -8741,8 +8748,8 @@
       <c r="S87" s="10"/>
     </row>
     <row r="88" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A88" s="185"/>
-      <c r="B88" s="175"/>
+      <c r="A88" s="186"/>
+      <c r="B88" s="176"/>
       <c r="C88" s="30" t="s">
         <v>151</v>
       </c>
@@ -8766,8 +8773,8 @@
       <c r="S88" s="10"/>
     </row>
     <row r="89" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A89" s="185"/>
-      <c r="B89" s="175"/>
+      <c r="A89" s="186"/>
+      <c r="B89" s="176"/>
       <c r="C89" s="30" t="s">
         <v>560</v>
       </c>
@@ -8791,8 +8798,8 @@
       <c r="S89" s="10"/>
     </row>
     <row r="90" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A90" s="186"/>
-      <c r="B90" s="175"/>
+      <c r="A90" s="187"/>
+      <c r="B90" s="176"/>
       <c r="C90" s="30" t="s">
         <v>152</v>
       </c>
@@ -8816,10 +8823,10 @@
       <c r="S90" s="10"/>
     </row>
     <row r="91" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A91" s="184" t="s">
+      <c r="A91" s="185" t="s">
         <v>616</v>
       </c>
-      <c r="B91" s="182" t="s">
+      <c r="B91" s="183" t="s">
         <v>95</v>
       </c>
       <c r="C91" s="31" t="s">
@@ -8849,8 +8856,8 @@
       <c r="S91" s="10"/>
     </row>
     <row r="92" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A92" s="186"/>
-      <c r="B92" s="183"/>
+      <c r="A92" s="187"/>
+      <c r="B92" s="184"/>
       <c r="C92" s="31" t="s">
         <v>132</v>
       </c>
@@ -8897,10 +8904,10 @@
       <c r="S93" s="10"/>
     </row>
     <row r="94" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A94" s="184" t="s">
+      <c r="A94" s="185" t="s">
         <v>112</v>
       </c>
-      <c r="B94" s="173" t="s">
+      <c r="B94" s="174" t="s">
         <v>101</v>
       </c>
       <c r="C94" s="31" t="s">
@@ -8928,8 +8935,8 @@
       <c r="S94" s="10"/>
     </row>
     <row r="95" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A95" s="185"/>
-      <c r="B95" s="174"/>
+      <c r="A95" s="186"/>
+      <c r="B95" s="175"/>
       <c r="C95" s="31" t="s">
         <v>563</v>
       </c>
@@ -8955,7 +8962,7 @@
       <c r="S95" s="10"/>
     </row>
     <row r="96" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A96" s="186"/>
+      <c r="A96" s="187"/>
       <c r="B96" s="111" t="s">
         <v>561</v>
       </c>
@@ -8984,7 +8991,7 @@
       <c r="S96" s="10"/>
     </row>
     <row r="97" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A97" s="184" t="s">
+      <c r="A97" s="185" t="s">
         <v>617</v>
       </c>
       <c r="B97" s="29" t="s">
@@ -9015,7 +9022,7 @@
       <c r="S97" s="10"/>
     </row>
     <row r="98" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A98" s="185"/>
+      <c r="A98" s="186"/>
       <c r="B98" s="23" t="s">
         <v>266</v>
       </c>
@@ -9044,7 +9051,7 @@
       <c r="S98" s="10"/>
     </row>
     <row r="99" spans="1:19" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="186"/>
+      <c r="A99" s="187"/>
       <c r="B99" s="22" t="s">
         <v>265</v>
       </c>
@@ -9071,7 +9078,7 @@
       <c r="S99" s="10"/>
     </row>
     <row r="100" spans="1:19" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="184" t="s">
+      <c r="A100" s="185" t="s">
         <v>618</v>
       </c>
       <c r="B100" s="22" t="s">
@@ -9100,7 +9107,7 @@
       <c r="S100" s="10"/>
     </row>
     <row r="101" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A101" s="186"/>
+      <c r="A101" s="187"/>
       <c r="B101" s="22" t="s">
         <v>264</v>
       </c>
@@ -9148,7 +9155,7 @@
       <c r="S102" s="10"/>
     </row>
     <row r="103" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A103" s="184" t="s">
+      <c r="A103" s="185" t="s">
         <v>606</v>
       </c>
       <c r="B103" s="23" t="s">
@@ -9179,7 +9186,7 @@
       <c r="S103" s="10"/>
     </row>
     <row r="104" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A104" s="185"/>
+      <c r="A104" s="186"/>
       <c r="B104" s="23" t="s">
         <v>540</v>
       </c>
@@ -9208,7 +9215,7 @@
       <c r="S104" s="10"/>
     </row>
     <row r="105" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A105" s="185"/>
+      <c r="A105" s="186"/>
       <c r="B105" s="23" t="s">
         <v>541</v>
       </c>
@@ -9237,8 +9244,8 @@
       <c r="S105" s="10"/>
     </row>
     <row r="106" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A106" s="185"/>
-      <c r="B106" s="170" t="s">
+      <c r="A106" s="186"/>
+      <c r="B106" s="171" t="s">
         <v>542</v>
       </c>
       <c r="C106" s="31" t="s">
@@ -9266,8 +9273,8 @@
       <c r="S106" s="10"/>
     </row>
     <row r="107" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A107" s="185"/>
-      <c r="B107" s="171"/>
+      <c r="A107" s="186"/>
+      <c r="B107" s="172"/>
       <c r="C107" s="31" t="s">
         <v>194</v>
       </c>
@@ -9293,8 +9300,8 @@
       <c r="S107" s="10"/>
     </row>
     <row r="108" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A108" s="185"/>
-      <c r="B108" s="172"/>
+      <c r="A108" s="186"/>
+      <c r="B108" s="173"/>
       <c r="C108" s="30" t="s">
         <v>195</v>
       </c>
@@ -9317,8 +9324,8 @@
       <c r="S108" s="10"/>
     </row>
     <row r="109" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A109" s="185"/>
-      <c r="B109" s="173" t="s">
+      <c r="A109" s="186"/>
+      <c r="B109" s="174" t="s">
         <v>543</v>
       </c>
       <c r="C109" s="31" t="s">
@@ -9346,8 +9353,8 @@
       <c r="S109" s="10"/>
     </row>
     <row r="110" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A110" s="185"/>
-      <c r="B110" s="174"/>
+      <c r="A110" s="186"/>
+      <c r="B110" s="175"/>
       <c r="C110" s="31" t="s">
         <v>548</v>
       </c>
@@ -9373,7 +9380,7 @@
       <c r="S110" s="10"/>
     </row>
     <row r="111" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A111" s="185"/>
+      <c r="A111" s="186"/>
       <c r="B111" s="23" t="s">
         <v>544</v>
       </c>
@@ -9402,8 +9409,8 @@
       <c r="S111" s="10"/>
     </row>
     <row r="112" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A112" s="185"/>
-      <c r="B112" s="173" t="s">
+      <c r="A112" s="186"/>
+      <c r="B112" s="174" t="s">
         <v>545</v>
       </c>
       <c r="C112" s="31" t="s">
@@ -9431,8 +9438,8 @@
       <c r="S112" s="10"/>
     </row>
     <row r="113" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A113" s="185"/>
-      <c r="B113" s="174"/>
+      <c r="A113" s="186"/>
+      <c r="B113" s="175"/>
       <c r="C113" s="31" t="s">
         <v>571</v>
       </c>
@@ -9458,7 +9465,7 @@
       <c r="S113" s="10"/>
     </row>
     <row r="114" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A114" s="186"/>
+      <c r="A114" s="187"/>
       <c r="B114" s="23" t="s">
         <v>546</v>
       </c>
@@ -9487,10 +9494,10 @@
       <c r="S114" s="10"/>
     </row>
     <row r="116" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B116" s="178" t="s">
+      <c r="B116" s="179" t="s">
         <v>245</v>
       </c>
-      <c r="C116" s="178"/>
+      <c r="C116" s="179"/>
       <c r="D116" s="68"/>
       <c r="E116" s="65"/>
       <c r="F116" s="65"/>
@@ -9507,19 +9514,19 @@
       <c r="S116" s="68"/>
     </row>
     <row r="117" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B117" s="165" t="s">
+      <c r="B117" s="166" t="s">
         <v>525</v>
       </c>
-      <c r="C117" s="165"/>
+      <c r="C117" s="166"/>
       <c r="D117" s="66"/>
       <c r="E117" s="66"/>
       <c r="F117" s="66"/>
     </row>
     <row r="118" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B118" s="166" t="s">
+      <c r="B118" s="167" t="s">
         <v>526</v>
       </c>
-      <c r="C118" s="166"/>
+      <c r="C118" s="167"/>
       <c r="D118" s="67"/>
       <c r="E118" s="67"/>
       <c r="F118" s="67"/>
@@ -9601,74 +9608,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:57" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D1" s="194" t="s">
+      <c r="D1" s="195" t="s">
         <v>622</v>
       </c>
-      <c r="E1" s="195"/>
-      <c r="F1" s="195"/>
-      <c r="G1" s="195"/>
-      <c r="H1" s="195"/>
-      <c r="I1" s="195"/>
-      <c r="J1" s="195"/>
-      <c r="K1" s="195"/>
-      <c r="L1" s="196"/>
+      <c r="E1" s="196"/>
+      <c r="F1" s="196"/>
+      <c r="G1" s="196"/>
+      <c r="H1" s="196"/>
+      <c r="I1" s="196"/>
+      <c r="J1" s="196"/>
+      <c r="K1" s="196"/>
+      <c r="L1" s="197"/>
       <c r="M1" s="6"/>
-      <c r="N1" s="197" t="s">
+      <c r="N1" s="198" t="s">
         <v>607</v>
       </c>
-      <c r="O1" s="198"/>
-      <c r="P1" s="199"/>
+      <c r="O1" s="199"/>
+      <c r="P1" s="200"/>
       <c r="Q1" s="6"/>
-      <c r="R1" s="191" t="s">
+      <c r="R1" s="192" t="s">
         <v>614</v>
       </c>
-      <c r="S1" s="192"/>
-      <c r="T1" s="192"/>
-      <c r="U1" s="192"/>
-      <c r="V1" s="192"/>
-      <c r="W1" s="192"/>
-      <c r="X1" s="193"/>
+      <c r="S1" s="193"/>
+      <c r="T1" s="193"/>
+      <c r="U1" s="193"/>
+      <c r="V1" s="193"/>
+      <c r="W1" s="193"/>
+      <c r="X1" s="194"/>
       <c r="Y1" s="6"/>
-      <c r="Z1" s="191" t="s">
+      <c r="Z1" s="192" t="s">
         <v>605</v>
       </c>
-      <c r="AA1" s="192"/>
-      <c r="AB1" s="192"/>
-      <c r="AC1" s="192"/>
-      <c r="AD1" s="192"/>
-      <c r="AE1" s="192"/>
-      <c r="AF1" s="193"/>
-      <c r="AG1" s="191" t="s">
+      <c r="AA1" s="193"/>
+      <c r="AB1" s="193"/>
+      <c r="AC1" s="193"/>
+      <c r="AD1" s="193"/>
+      <c r="AE1" s="193"/>
+      <c r="AF1" s="194"/>
+      <c r="AG1" s="192" t="s">
         <v>623</v>
       </c>
-      <c r="AH1" s="192"/>
-      <c r="AI1" s="192"/>
-      <c r="AJ1" s="192"/>
-      <c r="AK1" s="192"/>
-      <c r="AL1" s="192"/>
-      <c r="AM1" s="192"/>
-      <c r="AN1" s="193"/>
+      <c r="AH1" s="193"/>
+      <c r="AI1" s="193"/>
+      <c r="AJ1" s="193"/>
+      <c r="AK1" s="193"/>
+      <c r="AL1" s="193"/>
+      <c r="AM1" s="193"/>
+      <c r="AN1" s="194"/>
       <c r="AO1" s="6"/>
-      <c r="AP1" s="191" t="s">
+      <c r="AP1" s="192" t="s">
         <v>621</v>
       </c>
-      <c r="AQ1" s="192"/>
-      <c r="AR1" s="192"/>
-      <c r="AS1" s="192"/>
-      <c r="AT1" s="192"/>
-      <c r="AU1" s="192"/>
-      <c r="AV1" s="193"/>
+      <c r="AQ1" s="193"/>
+      <c r="AR1" s="193"/>
+      <c r="AS1" s="193"/>
+      <c r="AT1" s="193"/>
+      <c r="AU1" s="193"/>
+      <c r="AV1" s="194"/>
       <c r="AW1" s="6"/>
-      <c r="AX1" s="191" t="s">
+      <c r="AX1" s="192" t="s">
         <v>606</v>
       </c>
-      <c r="AY1" s="192"/>
-      <c r="AZ1" s="192"/>
-      <c r="BA1" s="192"/>
-      <c r="BB1" s="192"/>
-      <c r="BC1" s="192"/>
-      <c r="BD1" s="192"/>
-      <c r="BE1" s="193"/>
+      <c r="AY1" s="193"/>
+      <c r="AZ1" s="193"/>
+      <c r="BA1" s="193"/>
+      <c r="BB1" s="193"/>
+      <c r="BC1" s="193"/>
+      <c r="BD1" s="193"/>
+      <c r="BE1" s="194"/>
     </row>
     <row r="2" spans="1:57" ht="105" x14ac:dyDescent="0.2">
       <c r="A2" s="105" t="s">
@@ -9834,7 +9841,7 @@
       </c>
     </row>
     <row r="3" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="190" t="s">
+      <c r="A3" s="191" t="s">
         <v>236</v>
       </c>
       <c r="B3" s="53">
@@ -9899,7 +9906,7 @@
       <c r="BE3" s="25"/>
     </row>
     <row r="4" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="190"/>
+      <c r="A4" s="191"/>
       <c r="B4" s="53">
         <v>2</v>
       </c>
@@ -9962,7 +9969,7 @@
       <c r="BE4" s="25"/>
     </row>
     <row r="5" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="190"/>
+      <c r="A5" s="191"/>
       <c r="B5" s="54">
         <v>3</v>
       </c>
@@ -10028,7 +10035,7 @@
       <c r="BE5" s="25"/>
     </row>
     <row r="6" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="190"/>
+      <c r="A6" s="191"/>
       <c r="B6" s="54">
         <v>4</v>
       </c>
@@ -10090,7 +10097,7 @@
       <c r="BE6" s="25"/>
     </row>
     <row r="7" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="190"/>
+      <c r="A7" s="191"/>
       <c r="B7" s="53">
         <v>5</v>
       </c>
@@ -10153,7 +10160,7 @@
       <c r="BE7" s="25"/>
     </row>
     <row r="8" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="190"/>
+      <c r="A8" s="191"/>
       <c r="B8" s="54">
         <v>6</v>
       </c>
@@ -10218,7 +10225,7 @@
       <c r="BE8" s="25"/>
     </row>
     <row r="9" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="190"/>
+      <c r="A9" s="191"/>
       <c r="B9" s="54">
         <v>7</v>
       </c>
@@ -10289,7 +10296,7 @@
       <c r="BE9" s="25"/>
     </row>
     <row r="10" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="190"/>
+      <c r="A10" s="191"/>
       <c r="B10" s="55">
         <v>8</v>
       </c>
@@ -10356,7 +10363,7 @@
       <c r="BE10" s="25"/>
     </row>
     <row r="11" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="190"/>
+      <c r="A11" s="191"/>
       <c r="B11" s="54">
         <v>9</v>
       </c>
@@ -10421,7 +10428,7 @@
       <c r="BE11" s="25"/>
     </row>
     <row r="12" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="190"/>
+      <c r="A12" s="191"/>
       <c r="B12" s="54">
         <v>10</v>
       </c>
@@ -10547,7 +10554,7 @@
       <c r="BE13" s="10"/>
     </row>
     <row r="14" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="190" t="s">
+      <c r="A14" s="191" t="s">
         <v>241</v>
       </c>
       <c r="B14" s="54">
@@ -10616,7 +10623,7 @@
       <c r="BE14" s="25"/>
     </row>
     <row r="15" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="190"/>
+      <c r="A15" s="191"/>
       <c r="B15" s="53">
         <v>2</v>
       </c>
@@ -10738,7 +10745,7 @@
       <c r="BE16" s="10"/>
     </row>
     <row r="17" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="190" t="s">
+      <c r="A17" s="191" t="s">
         <v>237</v>
       </c>
       <c r="B17" s="55">
@@ -10808,7 +10815,7 @@
       <c r="BE17" s="25"/>
     </row>
     <row r="18" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="190"/>
+      <c r="A18" s="191"/>
       <c r="B18" s="55">
         <v>2</v>
       </c>
@@ -10877,7 +10884,7 @@
       <c r="BE18" s="25"/>
     </row>
     <row r="19" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="190"/>
+      <c r="A19" s="191"/>
       <c r="B19" s="56">
         <v>3</v>
       </c>
@@ -10940,7 +10947,7 @@
       <c r="BE19" s="25"/>
     </row>
     <row r="20" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="190"/>
+      <c r="A20" s="191"/>
       <c r="B20" s="55">
         <v>4</v>
       </c>
@@ -11023,7 +11030,7 @@
       </c>
     </row>
     <row r="21" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="190"/>
+      <c r="A21" s="191"/>
       <c r="B21" s="56">
         <v>5</v>
       </c>
@@ -11145,7 +11152,7 @@
       <c r="BE22" s="10"/>
     </row>
     <row r="23" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="187" t="s">
+      <c r="A23" s="188" t="s">
         <v>238</v>
       </c>
       <c r="B23" s="55">
@@ -11212,7 +11219,7 @@
       <c r="BE23" s="25"/>
     </row>
     <row r="24" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="188"/>
+      <c r="A24" s="189"/>
       <c r="B24" s="56">
         <v>2</v>
       </c>
@@ -11275,7 +11282,7 @@
       <c r="BE24" s="25"/>
     </row>
     <row r="25" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="188"/>
+      <c r="A25" s="189"/>
       <c r="B25" s="56">
         <v>3</v>
       </c>
@@ -11338,7 +11345,7 @@
       <c r="BE25" s="25"/>
     </row>
     <row r="26" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="188"/>
+      <c r="A26" s="189"/>
       <c r="B26" s="56">
         <v>4</v>
       </c>
@@ -11401,7 +11408,7 @@
       <c r="BE26" s="25"/>
     </row>
     <row r="27" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="188"/>
+      <c r="A27" s="189"/>
       <c r="B27" s="56">
         <v>5</v>
       </c>
@@ -11464,7 +11471,7 @@
       <c r="BE27" s="25"/>
     </row>
     <row r="28" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="188"/>
+      <c r="A28" s="189"/>
       <c r="B28" s="56">
         <v>6</v>
       </c>
@@ -11527,7 +11534,7 @@
       <c r="BE28" s="25"/>
     </row>
     <row r="29" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="188"/>
+      <c r="A29" s="189"/>
       <c r="B29" s="56">
         <v>7</v>
       </c>
@@ -11590,7 +11597,7 @@
       <c r="BE29" s="25"/>
     </row>
     <row r="30" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="188"/>
+      <c r="A30" s="189"/>
       <c r="B30" s="56">
         <v>8</v>
       </c>
@@ -11653,7 +11660,7 @@
       <c r="BE30" s="25"/>
     </row>
     <row r="31" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="188"/>
+      <c r="A31" s="189"/>
       <c r="B31" s="56">
         <v>9</v>
       </c>
@@ -11716,7 +11723,7 @@
       <c r="BE31" s="25"/>
     </row>
     <row r="32" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="188"/>
+      <c r="A32" s="189"/>
       <c r="B32" s="56">
         <v>10</v>
       </c>
@@ -11779,7 +11786,7 @@
       <c r="BE32" s="25"/>
     </row>
     <row r="33" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="189"/>
+      <c r="A33" s="190"/>
       <c r="B33" s="55">
         <v>11</v>
       </c>
@@ -11903,7 +11910,7 @@
       <c r="BE34" s="10"/>
     </row>
     <row r="35" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="187" t="s">
+      <c r="A35" s="188" t="s">
         <v>239</v>
       </c>
       <c r="B35" s="56">
@@ -11970,7 +11977,7 @@
       <c r="BE35" s="25"/>
     </row>
     <row r="36" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="188"/>
+      <c r="A36" s="189"/>
       <c r="B36" s="55">
         <v>2</v>
       </c>
@@ -12039,7 +12046,7 @@
       <c r="BE36" s="25"/>
     </row>
     <row r="37" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="188"/>
+      <c r="A37" s="189"/>
       <c r="B37" s="55">
         <v>3</v>
       </c>
@@ -12108,7 +12115,7 @@
       <c r="BE37" s="25"/>
     </row>
     <row r="38" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="189"/>
+      <c r="A38" s="190"/>
       <c r="B38" s="55">
         <v>4</v>
       </c>
@@ -12234,7 +12241,7 @@
       <c r="BE39" s="10"/>
     </row>
     <row r="40" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="190" t="s">
+      <c r="A40" s="191" t="s">
         <v>240</v>
       </c>
       <c r="B40" s="55">
@@ -12301,7 +12308,7 @@
       <c r="BE40" s="25"/>
     </row>
     <row r="41" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="190"/>
+      <c r="A41" s="191"/>
       <c r="B41" s="56">
         <v>2</v>
       </c>
@@ -12364,7 +12371,7 @@
       <c r="BE41" s="25"/>
     </row>
     <row r="42" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="190"/>
+      <c r="A42" s="191"/>
       <c r="B42" s="56">
         <v>3</v>
       </c>
@@ -12486,7 +12493,7 @@
       <c r="BE43" s="10"/>
     </row>
     <row r="44" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="187" t="s">
+      <c r="A44" s="188" t="s">
         <v>246</v>
       </c>
       <c r="B44" s="55">
@@ -12561,7 +12568,7 @@
       <c r="BE44" s="25"/>
     </row>
     <row r="45" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A45" s="188"/>
+      <c r="A45" s="189"/>
       <c r="B45" s="55">
         <v>2</v>
       </c>
@@ -12632,7 +12639,7 @@
       <c r="BE45" s="25"/>
     </row>
     <row r="46" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" s="188"/>
+      <c r="A46" s="189"/>
       <c r="B46" s="55">
         <v>3</v>
       </c>
@@ -12703,7 +12710,7 @@
       <c r="BE46" s="25"/>
     </row>
     <row r="47" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" s="189"/>
+      <c r="A47" s="190"/>
       <c r="B47" s="56">
         <v>4</v>
       </c>
@@ -12960,7 +12967,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB89FBCC-C415-8947-9B16-FD60E8EE8478}">
   <dimension ref="A1:BG60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
@@ -12986,74 +12993,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:59" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D1" s="194" t="s">
+      <c r="D1" s="195" t="s">
         <v>622</v>
       </c>
-      <c r="E1" s="195"/>
-      <c r="F1" s="195"/>
-      <c r="G1" s="195"/>
-      <c r="H1" s="195"/>
-      <c r="I1" s="195"/>
-      <c r="J1" s="195"/>
-      <c r="K1" s="195"/>
-      <c r="L1" s="196"/>
+      <c r="E1" s="196"/>
+      <c r="F1" s="196"/>
+      <c r="G1" s="196"/>
+      <c r="H1" s="196"/>
+      <c r="I1" s="196"/>
+      <c r="J1" s="196"/>
+      <c r="K1" s="196"/>
+      <c r="L1" s="197"/>
       <c r="M1" s="6"/>
-      <c r="N1" s="197" t="s">
+      <c r="N1" s="198" t="s">
         <v>607</v>
       </c>
-      <c r="O1" s="198"/>
-      <c r="P1" s="199"/>
+      <c r="O1" s="199"/>
+      <c r="P1" s="200"/>
       <c r="Q1" s="6"/>
-      <c r="R1" s="191" t="s">
+      <c r="R1" s="192" t="s">
         <v>614</v>
       </c>
-      <c r="S1" s="192"/>
-      <c r="T1" s="192"/>
-      <c r="U1" s="192"/>
-      <c r="V1" s="192"/>
-      <c r="W1" s="192"/>
-      <c r="X1" s="193"/>
+      <c r="S1" s="193"/>
+      <c r="T1" s="193"/>
+      <c r="U1" s="193"/>
+      <c r="V1" s="193"/>
+      <c r="W1" s="193"/>
+      <c r="X1" s="194"/>
       <c r="Y1" s="6"/>
-      <c r="Z1" s="191" t="s">
+      <c r="Z1" s="192" t="s">
         <v>605</v>
       </c>
-      <c r="AA1" s="192"/>
-      <c r="AB1" s="192"/>
-      <c r="AC1" s="192"/>
-      <c r="AD1" s="192"/>
-      <c r="AE1" s="192"/>
-      <c r="AF1" s="193"/>
-      <c r="AG1" s="191" t="s">
+      <c r="AA1" s="193"/>
+      <c r="AB1" s="193"/>
+      <c r="AC1" s="193"/>
+      <c r="AD1" s="193"/>
+      <c r="AE1" s="193"/>
+      <c r="AF1" s="194"/>
+      <c r="AG1" s="192" t="s">
         <v>623</v>
       </c>
-      <c r="AH1" s="192"/>
-      <c r="AI1" s="192"/>
-      <c r="AJ1" s="192"/>
-      <c r="AK1" s="192"/>
-      <c r="AL1" s="192"/>
-      <c r="AM1" s="192"/>
-      <c r="AN1" s="193"/>
+      <c r="AH1" s="193"/>
+      <c r="AI1" s="193"/>
+      <c r="AJ1" s="193"/>
+      <c r="AK1" s="193"/>
+      <c r="AL1" s="193"/>
+      <c r="AM1" s="193"/>
+      <c r="AN1" s="194"/>
       <c r="AO1" s="6"/>
-      <c r="AP1" s="191" t="s">
+      <c r="AP1" s="192" t="s">
         <v>621</v>
       </c>
-      <c r="AQ1" s="192"/>
-      <c r="AR1" s="192"/>
-      <c r="AS1" s="192"/>
-      <c r="AT1" s="192"/>
-      <c r="AU1" s="192"/>
-      <c r="AV1" s="193"/>
+      <c r="AQ1" s="193"/>
+      <c r="AR1" s="193"/>
+      <c r="AS1" s="193"/>
+      <c r="AT1" s="193"/>
+      <c r="AU1" s="193"/>
+      <c r="AV1" s="194"/>
       <c r="AW1" s="6"/>
-      <c r="AX1" s="191" t="s">
+      <c r="AX1" s="192" t="s">
         <v>606</v>
       </c>
-      <c r="AY1" s="192"/>
-      <c r="AZ1" s="192"/>
-      <c r="BA1" s="192"/>
-      <c r="BB1" s="192"/>
-      <c r="BC1" s="192"/>
-      <c r="BD1" s="192"/>
-      <c r="BE1" s="193"/>
+      <c r="AY1" s="193"/>
+      <c r="AZ1" s="193"/>
+      <c r="BA1" s="193"/>
+      <c r="BB1" s="193"/>
+      <c r="BC1" s="193"/>
+      <c r="BD1" s="193"/>
+      <c r="BE1" s="194"/>
     </row>
     <row r="2" spans="1:59" ht="105" x14ac:dyDescent="0.2">
       <c r="A2" s="105" t="s">
@@ -13219,10 +13226,10 @@
       </c>
     </row>
     <row r="3" spans="1:59" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="190" t="s">
+      <c r="A3" s="191" t="s">
         <v>236</v>
       </c>
-      <c r="B3" s="202">
+      <c r="B3" s="203">
         <v>1</v>
       </c>
       <c r="C3" s="15" t="s">
@@ -13284,8 +13291,8 @@
       <c r="BE3" s="25"/>
     </row>
     <row r="4" spans="1:59" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="190"/>
-      <c r="B4" s="203"/>
+      <c r="A4" s="191"/>
+      <c r="B4" s="204"/>
       <c r="C4" s="15" t="s">
         <v>508</v>
       </c>
@@ -13345,7 +13352,7 @@
       <c r="BE4" s="25"/>
     </row>
     <row r="5" spans="1:59" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="190"/>
+      <c r="A5" s="191"/>
       <c r="B5" s="53">
         <v>2</v>
       </c>
@@ -13408,7 +13415,7 @@
       <c r="BE5" s="25"/>
     </row>
     <row r="6" spans="1:59" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="190"/>
+      <c r="A6" s="191"/>
       <c r="B6" s="54">
         <v>3</v>
       </c>
@@ -13475,8 +13482,8 @@
       <c r="BE6" s="25"/>
     </row>
     <row r="7" spans="1:59" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="190"/>
-      <c r="B7" s="200">
+      <c r="A7" s="191"/>
+      <c r="B7" s="201">
         <v>4</v>
       </c>
       <c r="C7" s="15" t="s">
@@ -13538,8 +13545,8 @@
       <c r="BE7" s="25"/>
     </row>
     <row r="8" spans="1:59" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="190"/>
-      <c r="B8" s="201"/>
+      <c r="A8" s="191"/>
+      <c r="B8" s="202"/>
       <c r="C8" s="15" t="s">
         <v>394</v>
       </c>
@@ -13599,7 +13606,7 @@
       <c r="BE8" s="25"/>
     </row>
     <row r="9" spans="1:59" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="190"/>
+      <c r="A9" s="191"/>
       <c r="B9" s="53">
         <v>5</v>
       </c>
@@ -13662,7 +13669,7 @@
       <c r="BE9" s="25"/>
     </row>
     <row r="10" spans="1:59" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="190"/>
+      <c r="A10" s="191"/>
       <c r="B10" s="54">
         <v>6</v>
       </c>
@@ -13730,8 +13737,8 @@
       </c>
     </row>
     <row r="11" spans="1:59" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="190"/>
-      <c r="B11" s="200">
+      <c r="A11" s="191"/>
+      <c r="B11" s="201">
         <v>7</v>
       </c>
       <c r="C11" s="15" t="s">
@@ -13797,8 +13804,8 @@
       <c r="BE11" s="25"/>
     </row>
     <row r="12" spans="1:59" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="190"/>
-      <c r="B12" s="204"/>
+      <c r="A12" s="191"/>
+      <c r="B12" s="205"/>
       <c r="C12" s="15" t="s">
         <v>397</v>
       </c>
@@ -13870,7 +13877,7 @@
       <c r="BE12" s="25"/>
     </row>
     <row r="13" spans="1:59" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="190"/>
+      <c r="A13" s="191"/>
       <c r="B13" s="55">
         <v>8</v>
       </c>
@@ -13937,7 +13944,7 @@
       <c r="BE13" s="25"/>
     </row>
     <row r="14" spans="1:59" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="190"/>
+      <c r="A14" s="191"/>
       <c r="B14" s="54">
         <v>9</v>
       </c>
@@ -14002,7 +14009,7 @@
       <c r="BE14" s="25"/>
     </row>
     <row r="15" spans="1:59" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="190"/>
+      <c r="A15" s="191"/>
       <c r="B15" s="54">
         <v>10</v>
       </c>
@@ -14128,10 +14135,10 @@
       <c r="BE16" s="10"/>
     </row>
     <row r="17" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="190" t="s">
+      <c r="A17" s="191" t="s">
         <v>241</v>
       </c>
-      <c r="B17" s="200">
+      <c r="B17" s="201">
         <v>1</v>
       </c>
       <c r="C17" s="15" t="s">
@@ -14195,8 +14202,8 @@
       <c r="BE17" s="25"/>
     </row>
     <row r="18" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="190"/>
-      <c r="B18" s="201"/>
+      <c r="A18" s="191"/>
+      <c r="B18" s="202"/>
       <c r="C18" s="15" t="s">
         <v>402</v>
       </c>
@@ -14260,7 +14267,7 @@
       <c r="BE18" s="25"/>
     </row>
     <row r="19" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="190"/>
+      <c r="A19" s="191"/>
       <c r="B19" s="63">
         <v>2</v>
       </c>
@@ -14382,7 +14389,7 @@
       <c r="BE20" s="10"/>
     </row>
     <row r="21" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="190" t="s">
+      <c r="A21" s="191" t="s">
         <v>237</v>
       </c>
       <c r="B21" s="55">
@@ -14452,7 +14459,7 @@
       <c r="BE21" s="25"/>
     </row>
     <row r="22" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="190"/>
+      <c r="A22" s="191"/>
       <c r="B22" s="55">
         <v>2</v>
       </c>
@@ -14519,7 +14526,7 @@
       <c r="BE22" s="25"/>
     </row>
     <row r="23" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="190"/>
+      <c r="A23" s="191"/>
       <c r="B23" s="56">
         <v>3</v>
       </c>
@@ -14582,8 +14589,8 @@
       <c r="BE23" s="25"/>
     </row>
     <row r="24" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="190"/>
-      <c r="B24" s="208">
+      <c r="A24" s="191"/>
+      <c r="B24" s="209">
         <v>4</v>
       </c>
       <c r="C24" s="17" t="s">
@@ -14647,8 +14654,8 @@
       <c r="BE24" s="25"/>
     </row>
     <row r="25" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="190"/>
-      <c r="B25" s="209"/>
+      <c r="A25" s="191"/>
+      <c r="B25" s="210"/>
       <c r="C25" s="17" t="s">
         <v>405</v>
       </c>
@@ -14718,8 +14725,8 @@
       <c r="BE25" s="25"/>
     </row>
     <row r="26" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="190"/>
-      <c r="B26" s="210"/>
+      <c r="A26" s="191"/>
+      <c r="B26" s="211"/>
       <c r="C26" s="17" t="s">
         <v>406</v>
       </c>
@@ -14789,7 +14796,7 @@
       </c>
     </row>
     <row r="27" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="190"/>
+      <c r="A27" s="191"/>
       <c r="B27" s="64">
         <v>5</v>
       </c>
@@ -14911,7 +14918,7 @@
       <c r="BE28" s="10"/>
     </row>
     <row r="29" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="211" t="s">
+      <c r="A29" s="212" t="s">
         <v>238</v>
       </c>
       <c r="B29" s="55">
@@ -14978,7 +14985,7 @@
       <c r="BE29" s="25"/>
     </row>
     <row r="30" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="212"/>
+      <c r="A30" s="213"/>
       <c r="B30" s="56">
         <v>2</v>
       </c>
@@ -15041,7 +15048,7 @@
       <c r="BE30" s="25"/>
     </row>
     <row r="31" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="212"/>
+      <c r="A31" s="213"/>
       <c r="B31" s="56">
         <v>3</v>
       </c>
@@ -15104,7 +15111,7 @@
       <c r="BE31" s="25"/>
     </row>
     <row r="32" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="212"/>
+      <c r="A32" s="213"/>
       <c r="B32" s="56">
         <v>4</v>
       </c>
@@ -15167,7 +15174,7 @@
       <c r="BE32" s="25"/>
     </row>
     <row r="33" spans="1:57" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="212"/>
+      <c r="A33" s="213"/>
       <c r="B33" s="56">
         <v>5</v>
       </c>
@@ -15230,7 +15237,7 @@
       <c r="BE33" s="25"/>
     </row>
     <row r="34" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="212"/>
+      <c r="A34" s="213"/>
       <c r="B34" s="56">
         <v>6</v>
       </c>
@@ -15293,7 +15300,7 @@
       <c r="BE34" s="25"/>
     </row>
     <row r="35" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="212"/>
+      <c r="A35" s="213"/>
       <c r="B35" s="56">
         <v>7</v>
       </c>
@@ -15356,7 +15363,7 @@
       <c r="BE35" s="25"/>
     </row>
     <row r="36" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="212"/>
+      <c r="A36" s="213"/>
       <c r="B36" s="56">
         <v>8</v>
       </c>
@@ -15419,7 +15426,7 @@
       <c r="BE36" s="25"/>
     </row>
     <row r="37" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="212"/>
+      <c r="A37" s="213"/>
       <c r="B37" s="56">
         <v>9</v>
       </c>
@@ -15482,7 +15489,7 @@
       <c r="BE37" s="25"/>
     </row>
     <row r="38" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="212"/>
+      <c r="A38" s="213"/>
       <c r="B38" s="56">
         <v>10</v>
       </c>
@@ -15545,7 +15552,7 @@
       <c r="BE38" s="25"/>
     </row>
     <row r="39" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="213"/>
+      <c r="A39" s="214"/>
       <c r="B39" s="121">
         <v>11</v>
       </c>
@@ -15669,7 +15676,7 @@
       <c r="BE40" s="10"/>
     </row>
     <row r="41" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="187" t="s">
+      <c r="A41" s="188" t="s">
         <v>239</v>
       </c>
       <c r="B41" s="56">
@@ -15736,7 +15743,7 @@
       <c r="BE41" s="25"/>
     </row>
     <row r="42" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="188"/>
+      <c r="A42" s="189"/>
       <c r="B42" s="55">
         <v>2</v>
       </c>
@@ -15805,7 +15812,7 @@
       <c r="BE42" s="25"/>
     </row>
     <row r="43" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="188"/>
+      <c r="A43" s="189"/>
       <c r="B43" s="55">
         <v>3</v>
       </c>
@@ -15874,7 +15881,7 @@
       <c r="BE43" s="25"/>
     </row>
     <row r="44" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="189"/>
+      <c r="A44" s="190"/>
       <c r="B44" s="121">
         <v>4</v>
       </c>
@@ -16000,7 +16007,7 @@
       <c r="BE45" s="10"/>
     </row>
     <row r="46" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" s="190" t="s">
+      <c r="A46" s="191" t="s">
         <v>240</v>
       </c>
       <c r="B46" s="55">
@@ -16067,7 +16074,7 @@
       <c r="BE46" s="25"/>
     </row>
     <row r="47" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" s="190"/>
+      <c r="A47" s="191"/>
       <c r="B47" s="56">
         <v>2</v>
       </c>
@@ -16130,7 +16137,7 @@
       <c r="BE47" s="25"/>
     </row>
     <row r="48" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A48" s="190"/>
+      <c r="A48" s="191"/>
       <c r="B48" s="64">
         <v>3</v>
       </c>
@@ -16252,13 +16259,13 @@
       <c r="BE49" s="10"/>
     </row>
     <row r="50" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="187" t="s">
+      <c r="A50" s="188" t="s">
         <v>246</v>
       </c>
       <c r="B50" s="55">
         <v>1</v>
       </c>
-      <c r="C50" s="205" t="s">
+      <c r="C50" s="206" t="s">
         <v>420</v>
       </c>
       <c r="D50" s="11"/>
@@ -16327,11 +16334,11 @@
       <c r="BE50" s="25"/>
     </row>
     <row r="51" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="188"/>
+      <c r="A51" s="189"/>
       <c r="B51" s="55">
         <v>2</v>
       </c>
-      <c r="C51" s="206"/>
+      <c r="C51" s="207"/>
       <c r="D51" s="11"/>
       <c r="E51" s="25"/>
       <c r="F51" s="25"/>
@@ -16396,11 +16403,11 @@
       <c r="BE51" s="25"/>
     </row>
     <row r="52" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="188"/>
+      <c r="A52" s="189"/>
       <c r="B52" s="55">
         <v>3</v>
       </c>
-      <c r="C52" s="207"/>
+      <c r="C52" s="208"/>
       <c r="D52" s="11"/>
       <c r="E52" s="25"/>
       <c r="F52" s="25"/>
@@ -16465,7 +16472,7 @@
       <c r="BE52" s="25"/>
     </row>
     <row r="53" spans="1:57" ht="17" x14ac:dyDescent="0.2">
-      <c r="A53" s="189"/>
+      <c r="A53" s="190"/>
       <c r="B53" s="56">
         <v>4</v>
       </c>
@@ -16771,75 +16778,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:58" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="218"/>
-      <c r="B1" s="218"/>
-      <c r="C1" s="218"/>
-      <c r="D1" s="219"/>
-      <c r="E1" s="220" t="s">
+      <c r="A1" s="219"/>
+      <c r="B1" s="219"/>
+      <c r="C1" s="219"/>
+      <c r="D1" s="220"/>
+      <c r="E1" s="221" t="s">
         <v>236</v>
       </c>
-      <c r="F1" s="220"/>
-      <c r="G1" s="220"/>
-      <c r="H1" s="220"/>
-      <c r="I1" s="220"/>
-      <c r="J1" s="220"/>
-      <c r="K1" s="220"/>
-      <c r="L1" s="220"/>
-      <c r="M1" s="220"/>
-      <c r="N1" s="220"/>
-      <c r="O1" s="220"/>
-      <c r="P1" s="220"/>
-      <c r="Q1" s="220"/>
+      <c r="F1" s="221"/>
+      <c r="G1" s="221"/>
+      <c r="H1" s="221"/>
+      <c r="I1" s="221"/>
+      <c r="J1" s="221"/>
+      <c r="K1" s="221"/>
+      <c r="L1" s="221"/>
+      <c r="M1" s="221"/>
+      <c r="N1" s="221"/>
+      <c r="O1" s="221"/>
+      <c r="P1" s="221"/>
+      <c r="Q1" s="221"/>
       <c r="R1" s="97"/>
-      <c r="S1" s="220" t="s">
+      <c r="S1" s="221" t="s">
         <v>241</v>
       </c>
-      <c r="T1" s="220"/>
-      <c r="U1" s="220"/>
+      <c r="T1" s="221"/>
+      <c r="U1" s="221"/>
       <c r="V1" s="97"/>
-      <c r="W1" s="220" t="s">
+      <c r="W1" s="221" t="s">
         <v>237</v>
       </c>
-      <c r="X1" s="220"/>
-      <c r="Y1" s="220"/>
-      <c r="Z1" s="220"/>
-      <c r="AA1" s="220"/>
-      <c r="AB1" s="220"/>
-      <c r="AC1" s="220"/>
+      <c r="X1" s="221"/>
+      <c r="Y1" s="221"/>
+      <c r="Z1" s="221"/>
+      <c r="AA1" s="221"/>
+      <c r="AB1" s="221"/>
+      <c r="AC1" s="221"/>
       <c r="AD1" s="97"/>
-      <c r="AE1" s="235" t="s">
+      <c r="AE1" s="236" t="s">
         <v>238</v>
       </c>
-      <c r="AF1" s="236"/>
-      <c r="AG1" s="236"/>
-      <c r="AH1" s="236"/>
-      <c r="AI1" s="236"/>
-      <c r="AJ1" s="236"/>
-      <c r="AK1" s="236"/>
-      <c r="AL1" s="236"/>
-      <c r="AM1" s="236"/>
-      <c r="AN1" s="236"/>
-      <c r="AO1" s="237"/>
+      <c r="AF1" s="237"/>
+      <c r="AG1" s="237"/>
+      <c r="AH1" s="237"/>
+      <c r="AI1" s="237"/>
+      <c r="AJ1" s="237"/>
+      <c r="AK1" s="237"/>
+      <c r="AL1" s="237"/>
+      <c r="AM1" s="237"/>
+      <c r="AN1" s="237"/>
+      <c r="AO1" s="238"/>
       <c r="AP1" s="97"/>
-      <c r="AQ1" s="232" t="s">
+      <c r="AQ1" s="233" t="s">
         <v>239</v>
       </c>
-      <c r="AR1" s="233"/>
-      <c r="AS1" s="233"/>
-      <c r="AT1" s="234"/>
+      <c r="AR1" s="234"/>
+      <c r="AS1" s="234"/>
+      <c r="AT1" s="235"/>
       <c r="AU1" s="97"/>
-      <c r="AV1" s="220" t="s">
+      <c r="AV1" s="221" t="s">
         <v>240</v>
       </c>
-      <c r="AW1" s="220"/>
-      <c r="AX1" s="220"/>
+      <c r="AW1" s="221"/>
+      <c r="AX1" s="221"/>
       <c r="AY1" s="97"/>
-      <c r="AZ1" s="229" t="s">
+      <c r="AZ1" s="230" t="s">
         <v>246</v>
       </c>
-      <c r="BA1" s="230"/>
-      <c r="BB1" s="230"/>
-      <c r="BC1" s="231"/>
+      <c r="BA1" s="231"/>
+      <c r="BB1" s="231"/>
+      <c r="BC1" s="232"/>
       <c r="BD1" s="97"/>
       <c r="BE1" s="98" t="s">
         <v>234</v>
@@ -16849,34 +16856,34 @@
       </c>
     </row>
     <row r="2" spans="1:58" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="218"/>
-      <c r="B2" s="218"/>
-      <c r="C2" s="218"/>
-      <c r="D2" s="219"/>
-      <c r="E2" s="221">
+      <c r="A2" s="219"/>
+      <c r="B2" s="219"/>
+      <c r="C2" s="219"/>
+      <c r="D2" s="220"/>
+      <c r="E2" s="222">
         <v>1</v>
       </c>
-      <c r="F2" s="222"/>
+      <c r="F2" s="223"/>
       <c r="G2" s="42">
         <v>2</v>
       </c>
       <c r="H2" s="42">
         <v>3</v>
       </c>
-      <c r="I2" s="223">
+      <c r="I2" s="224">
         <v>4</v>
       </c>
-      <c r="J2" s="224"/>
+      <c r="J2" s="225"/>
       <c r="K2" s="41">
         <v>5</v>
       </c>
       <c r="L2" s="42">
         <v>6</v>
       </c>
-      <c r="M2" s="214">
+      <c r="M2" s="215">
         <v>7</v>
       </c>
-      <c r="N2" s="215"/>
+      <c r="N2" s="216"/>
       <c r="O2" s="23">
         <v>8</v>
       </c>
@@ -16887,10 +16894,10 @@
         <v>10</v>
       </c>
       <c r="R2" s="36"/>
-      <c r="S2" s="223">
+      <c r="S2" s="224">
         <v>1</v>
       </c>
-      <c r="T2" s="224"/>
+      <c r="T2" s="225"/>
       <c r="U2" s="49">
         <v>2</v>
       </c>
@@ -16904,11 +16911,11 @@
       <c r="Y2" s="24">
         <v>3</v>
       </c>
-      <c r="Z2" s="238">
+      <c r="Z2" s="239">
         <v>4</v>
       </c>
-      <c r="AA2" s="239"/>
-      <c r="AB2" s="240"/>
+      <c r="AA2" s="240"/>
+      <c r="AB2" s="241"/>
       <c r="AC2" s="50">
         <v>5</v>
       </c>
@@ -16988,10 +16995,10 @@
       </c>
     </row>
     <row r="3" spans="1:58" s="48" customFormat="1" ht="329" x14ac:dyDescent="0.2">
-      <c r="A3" s="218"/>
-      <c r="B3" s="218"/>
-      <c r="C3" s="218"/>
-      <c r="D3" s="219"/>
+      <c r="A3" s="219"/>
+      <c r="B3" s="219"/>
+      <c r="C3" s="219"/>
+      <c r="D3" s="220"/>
       <c r="E3" s="43" t="s">
         <v>391</v>
       </c>
@@ -17121,11 +17128,11 @@
         <v>630</v>
       </c>
       <c r="AY3" s="45"/>
-      <c r="AZ3" s="226" t="s">
+      <c r="AZ3" s="227" t="s">
         <v>420</v>
       </c>
-      <c r="BA3" s="227"/>
-      <c r="BB3" s="228"/>
+      <c r="BA3" s="228"/>
+      <c r="BB3" s="229"/>
       <c r="BC3" s="46" t="s">
         <v>421</v>
       </c>
@@ -17135,10 +17142,10 @@
       </c>
     </row>
     <row r="4" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A4" s="187" t="s">
+      <c r="A4" s="188" t="s">
         <v>613</v>
       </c>
-      <c r="B4" s="216" t="s">
+      <c r="B4" s="217" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="30" t="s">
@@ -17202,8 +17209,8 @@
       <c r="BE4" s="11"/>
     </row>
     <row r="5" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A5" s="188"/>
-      <c r="B5" s="225"/>
+      <c r="A5" s="189"/>
+      <c r="B5" s="226"/>
       <c r="C5" s="30" t="s">
         <v>155</v>
       </c>
@@ -17265,8 +17272,8 @@
       <c r="BE5" s="11"/>
     </row>
     <row r="6" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A6" s="188"/>
-      <c r="B6" s="225"/>
+      <c r="A6" s="189"/>
+      <c r="B6" s="226"/>
       <c r="C6" s="31" t="s">
         <v>156</v>
       </c>
@@ -17330,8 +17337,8 @@
       <c r="BE6" s="11"/>
     </row>
     <row r="7" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A7" s="188"/>
-      <c r="B7" s="225"/>
+      <c r="A7" s="189"/>
+      <c r="B7" s="226"/>
       <c r="C7" s="30" t="s">
         <v>157</v>
       </c>
@@ -17393,8 +17400,8 @@
       <c r="BE7" s="11"/>
     </row>
     <row r="8" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A8" s="188"/>
-      <c r="B8" s="225"/>
+      <c r="A8" s="189"/>
+      <c r="B8" s="226"/>
       <c r="C8" s="30" t="s">
         <v>158</v>
       </c>
@@ -17456,8 +17463,8 @@
       <c r="BE8" s="11"/>
     </row>
     <row r="9" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A9" s="188"/>
-      <c r="B9" s="225"/>
+      <c r="A9" s="189"/>
+      <c r="B9" s="226"/>
       <c r="C9" s="30" t="s">
         <v>159</v>
       </c>
@@ -17519,8 +17526,8 @@
       <c r="BE9" s="25"/>
     </row>
     <row r="10" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A10" s="188"/>
-      <c r="B10" s="225"/>
+      <c r="A10" s="189"/>
+      <c r="B10" s="226"/>
       <c r="C10" s="31" t="s">
         <v>161</v>
       </c>
@@ -17586,8 +17593,8 @@
       <c r="BE10" s="25"/>
     </row>
     <row r="11" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A11" s="188"/>
-      <c r="B11" s="225"/>
+      <c r="A11" s="189"/>
+      <c r="B11" s="226"/>
       <c r="C11" s="30" t="s">
         <v>162</v>
       </c>
@@ -17649,8 +17656,8 @@
       <c r="BE11" s="25"/>
     </row>
     <row r="12" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A12" s="188"/>
-      <c r="B12" s="217"/>
+      <c r="A12" s="189"/>
+      <c r="B12" s="218"/>
       <c r="C12" s="30" t="s">
         <v>163</v>
       </c>
@@ -17712,8 +17719,8 @@
       <c r="BE12" s="11"/>
     </row>
     <row r="13" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A13" s="188"/>
-      <c r="B13" s="216" t="s">
+      <c r="A13" s="189"/>
+      <c r="B13" s="217" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="31" t="s">
@@ -17781,8 +17788,8 @@
       <c r="BE13" s="9"/>
     </row>
     <row r="14" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A14" s="188"/>
-      <c r="B14" s="217"/>
+      <c r="A14" s="189"/>
+      <c r="B14" s="218"/>
       <c r="C14" s="30" t="s">
         <v>162</v>
       </c>
@@ -17844,8 +17851,8 @@
       <c r="BE14" s="9"/>
     </row>
     <row r="15" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A15" s="188"/>
-      <c r="B15" s="216" t="s">
+      <c r="A15" s="189"/>
+      <c r="B15" s="217" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="30" t="s">
@@ -17909,8 +17916,8 @@
       <c r="BE15" s="9"/>
     </row>
     <row r="16" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A16" s="188"/>
-      <c r="B16" s="225"/>
+      <c r="A16" s="189"/>
+      <c r="B16" s="226"/>
       <c r="C16" s="30" t="s">
         <v>160</v>
       </c>
@@ -17972,7 +17979,7 @@
       <c r="BE16" s="9"/>
     </row>
     <row r="17" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A17" s="188"/>
+      <c r="A17" s="189"/>
       <c r="B17" s="136" t="s">
         <v>6</v>
       </c>
@@ -18041,7 +18048,7 @@
       <c r="BE17" s="9"/>
     </row>
     <row r="18" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A18" s="189"/>
+      <c r="A18" s="190"/>
       <c r="B18" s="137" t="s">
         <v>7</v>
       </c>
@@ -18106,10 +18113,10 @@
       <c r="BE18" s="9"/>
     </row>
     <row r="19" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A19" s="187" t="s">
+      <c r="A19" s="188" t="s">
         <v>612</v>
       </c>
-      <c r="B19" s="216" t="s">
+      <c r="B19" s="217" t="s">
         <v>14</v>
       </c>
       <c r="C19" s="31" t="s">
@@ -18175,8 +18182,8 @@
       <c r="BE19" s="9"/>
     </row>
     <row r="20" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A20" s="188"/>
-      <c r="B20" s="225"/>
+      <c r="A20" s="189"/>
+      <c r="B20" s="226"/>
       <c r="C20" s="30" t="s">
         <v>167</v>
       </c>
@@ -18238,8 +18245,8 @@
       <c r="BE20" s="9"/>
     </row>
     <row r="21" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A21" s="188"/>
-      <c r="B21" s="225"/>
+      <c r="A21" s="189"/>
+      <c r="B21" s="226"/>
       <c r="C21" s="30" t="s">
         <v>169</v>
       </c>
@@ -18301,8 +18308,8 @@
       <c r="BE21" s="25"/>
     </row>
     <row r="22" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A22" s="188"/>
-      <c r="B22" s="225"/>
+      <c r="A22" s="189"/>
+      <c r="B22" s="226"/>
       <c r="C22" s="31" t="s">
         <v>169</v>
       </c>
@@ -18366,8 +18373,8 @@
       <c r="BE22" s="9"/>
     </row>
     <row r="23" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A23" s="188"/>
-      <c r="B23" s="225"/>
+      <c r="A23" s="189"/>
+      <c r="B23" s="226"/>
       <c r="C23" s="30" t="s">
         <v>170</v>
       </c>
@@ -18429,8 +18436,8 @@
       <c r="BE23" s="9"/>
     </row>
     <row r="24" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A24" s="188"/>
-      <c r="B24" s="225"/>
+      <c r="A24" s="189"/>
+      <c r="B24" s="226"/>
       <c r="C24" s="30" t="s">
         <v>171</v>
       </c>
@@ -18492,8 +18499,8 @@
       <c r="BE24" s="9"/>
     </row>
     <row r="25" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A25" s="188"/>
-      <c r="B25" s="225"/>
+      <c r="A25" s="189"/>
+      <c r="B25" s="226"/>
       <c r="C25" s="30" t="s">
         <v>172</v>
       </c>
@@ -18555,8 +18562,8 @@
       <c r="BE25" s="9"/>
     </row>
     <row r="26" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A26" s="188"/>
-      <c r="B26" s="225"/>
+      <c r="A26" s="189"/>
+      <c r="B26" s="226"/>
       <c r="C26" s="30" t="s">
         <v>173</v>
       </c>
@@ -18618,8 +18625,8 @@
       <c r="BE26" s="9"/>
     </row>
     <row r="27" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A27" s="188"/>
-      <c r="B27" s="225"/>
+      <c r="A27" s="189"/>
+      <c r="B27" s="226"/>
       <c r="C27" s="30" t="s">
         <v>174</v>
       </c>
@@ -18681,8 +18688,8 @@
       <c r="BE27" s="9"/>
     </row>
     <row r="28" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A28" s="188"/>
-      <c r="B28" s="225"/>
+      <c r="A28" s="189"/>
+      <c r="B28" s="226"/>
       <c r="C28" s="30" t="s">
         <v>175</v>
       </c>
@@ -18744,8 +18751,8 @@
       <c r="BE28" s="25"/>
     </row>
     <row r="29" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A29" s="188"/>
-      <c r="B29" s="225"/>
+      <c r="A29" s="189"/>
+      <c r="B29" s="226"/>
       <c r="C29" s="30" t="s">
         <v>176</v>
       </c>
@@ -18807,8 +18814,8 @@
       <c r="BE29" s="25"/>
     </row>
     <row r="30" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A30" s="188"/>
-      <c r="B30" s="225"/>
+      <c r="A30" s="189"/>
+      <c r="B30" s="226"/>
       <c r="C30" s="30" t="s">
         <v>177</v>
       </c>
@@ -18870,8 +18877,8 @@
       <c r="BE30" s="9"/>
     </row>
     <row r="31" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A31" s="188"/>
-      <c r="B31" s="225"/>
+      <c r="A31" s="189"/>
+      <c r="B31" s="226"/>
       <c r="C31" s="30" t="s">
         <v>178</v>
       </c>
@@ -18933,8 +18940,8 @@
       <c r="BE31" s="9"/>
     </row>
     <row r="32" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A32" s="188"/>
-      <c r="B32" s="225"/>
+      <c r="A32" s="189"/>
+      <c r="B32" s="226"/>
       <c r="C32" s="30" t="s">
         <v>179</v>
       </c>
@@ -18996,8 +19003,8 @@
       <c r="BE32" s="9"/>
     </row>
     <row r="33" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A33" s="188"/>
-      <c r="B33" s="225"/>
+      <c r="A33" s="189"/>
+      <c r="B33" s="226"/>
       <c r="C33" s="30" t="s">
         <v>180</v>
       </c>
@@ -19059,8 +19066,8 @@
       <c r="BE33" s="9"/>
     </row>
     <row r="34" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A34" s="188"/>
-      <c r="B34" s="225"/>
+      <c r="A34" s="189"/>
+      <c r="B34" s="226"/>
       <c r="C34" s="30" t="s">
         <v>181</v>
       </c>
@@ -19122,8 +19129,8 @@
       <c r="BE34" s="9"/>
     </row>
     <row r="35" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A35" s="188"/>
-      <c r="B35" s="225"/>
+      <c r="A35" s="189"/>
+      <c r="B35" s="226"/>
       <c r="C35" s="30" t="s">
         <v>182</v>
       </c>
@@ -19185,8 +19192,8 @@
       <c r="BE35" s="25"/>
     </row>
     <row r="36" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A36" s="188"/>
-      <c r="B36" s="225"/>
+      <c r="A36" s="189"/>
+      <c r="B36" s="226"/>
       <c r="C36" s="30" t="s">
         <v>183</v>
       </c>
@@ -19248,8 +19255,8 @@
       <c r="BE36" s="25"/>
     </row>
     <row r="37" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A37" s="188"/>
-      <c r="B37" s="225"/>
+      <c r="A37" s="189"/>
+      <c r="B37" s="226"/>
       <c r="C37" s="30" t="s">
         <v>184</v>
       </c>
@@ -19311,8 +19318,8 @@
       <c r="BE37" s="9"/>
     </row>
     <row r="38" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A38" s="188"/>
-      <c r="B38" s="217"/>
+      <c r="A38" s="189"/>
+      <c r="B38" s="218"/>
       <c r="C38" s="30" t="s">
         <v>185</v>
       </c>
@@ -19374,7 +19381,7 @@
       <c r="BE38" s="9"/>
     </row>
     <row r="39" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A39" s="188"/>
+      <c r="A39" s="189"/>
       <c r="B39" s="138" t="s">
         <v>15</v>
       </c>
@@ -19439,8 +19446,8 @@
       <c r="BE39" s="9"/>
     </row>
     <row r="40" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A40" s="188"/>
-      <c r="B40" s="182" t="s">
+      <c r="A40" s="189"/>
+      <c r="B40" s="183" t="s">
         <v>16</v>
       </c>
       <c r="C40" s="31" t="s">
@@ -19506,8 +19513,8 @@
       <c r="BE40" s="9"/>
     </row>
     <row r="41" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A41" s="188"/>
-      <c r="B41" s="242"/>
+      <c r="A41" s="189"/>
+      <c r="B41" s="243"/>
       <c r="C41" s="31" t="s">
         <v>188</v>
       </c>
@@ -19571,8 +19578,8 @@
       <c r="BE41" s="9"/>
     </row>
     <row r="42" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A42" s="188"/>
-      <c r="B42" s="242"/>
+      <c r="A42" s="189"/>
+      <c r="B42" s="243"/>
       <c r="C42" s="31" t="s">
         <v>189</v>
       </c>
@@ -19636,8 +19643,8 @@
       <c r="BE42" s="9"/>
     </row>
     <row r="43" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A43" s="188"/>
-      <c r="B43" s="242"/>
+      <c r="A43" s="189"/>
+      <c r="B43" s="243"/>
       <c r="C43" s="31" t="s">
         <v>190</v>
       </c>
@@ -19701,8 +19708,8 @@
       <c r="BE43" s="9"/>
     </row>
     <row r="44" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A44" s="188"/>
-      <c r="B44" s="242"/>
+      <c r="A44" s="189"/>
+      <c r="B44" s="243"/>
       <c r="C44" s="31" t="s">
         <v>191</v>
       </c>
@@ -19766,8 +19773,8 @@
       <c r="BE44" s="9"/>
     </row>
     <row r="45" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A45" s="188"/>
-      <c r="B45" s="242"/>
+      <c r="A45" s="189"/>
+      <c r="B45" s="243"/>
       <c r="C45" s="31" t="s">
         <v>581</v>
       </c>
@@ -19831,8 +19838,8 @@
       <c r="BE45" s="9"/>
     </row>
     <row r="46" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A46" s="188"/>
-      <c r="B46" s="242"/>
+      <c r="A46" s="189"/>
+      <c r="B46" s="243"/>
       <c r="C46" s="31" t="s">
         <v>552</v>
       </c>
@@ -19896,8 +19903,8 @@
       <c r="BE46" s="9"/>
     </row>
     <row r="47" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A47" s="188"/>
-      <c r="B47" s="183"/>
+      <c r="A47" s="189"/>
+      <c r="B47" s="184"/>
       <c r="C47" s="31" t="s">
         <v>553</v>
       </c>
@@ -19961,8 +19968,8 @@
       <c r="BE47" s="9"/>
     </row>
     <row r="48" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A48" s="188"/>
-      <c r="B48" s="182" t="s">
+      <c r="A48" s="189"/>
+      <c r="B48" s="183" t="s">
         <v>17</v>
       </c>
       <c r="C48" s="31" t="s">
@@ -20028,8 +20035,8 @@
       <c r="BE48" s="9"/>
     </row>
     <row r="49" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A49" s="189"/>
-      <c r="B49" s="183"/>
+      <c r="A49" s="190"/>
+      <c r="B49" s="184"/>
       <c r="C49" s="31" t="s">
         <v>555</v>
       </c>
@@ -20152,10 +20159,10 @@
       <c r="BE50" s="10"/>
     </row>
     <row r="51" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A51" s="184" t="s">
+      <c r="A51" s="185" t="s">
         <v>619</v>
       </c>
-      <c r="B51" s="243" t="s">
+      <c r="B51" s="244" t="s">
         <v>262</v>
       </c>
       <c r="C51" s="30" t="s">
@@ -20219,8 +20226,8 @@
       <c r="BE51" s="18"/>
     </row>
     <row r="52" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A52" s="185"/>
-      <c r="B52" s="244"/>
+      <c r="A52" s="186"/>
+      <c r="B52" s="245"/>
       <c r="C52" s="30" t="s">
         <v>126</v>
       </c>
@@ -20282,7 +20289,7 @@
       <c r="BE52" s="18"/>
     </row>
     <row r="53" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A53" s="185"/>
+      <c r="A53" s="186"/>
       <c r="B53" s="140" t="s">
         <v>263</v>
       </c>
@@ -20347,8 +20354,8 @@
       <c r="BE53" s="18"/>
     </row>
     <row r="54" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A54" s="185"/>
-      <c r="B54" s="216" t="s">
+      <c r="A54" s="186"/>
+      <c r="B54" s="217" t="s">
         <v>23</v>
       </c>
       <c r="C54" s="30" t="s">
@@ -20412,8 +20419,8 @@
       <c r="BE54" s="9"/>
     </row>
     <row r="55" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A55" s="185"/>
-      <c r="B55" s="225"/>
+      <c r="A55" s="186"/>
+      <c r="B55" s="226"/>
       <c r="C55" s="30" t="s">
         <v>251</v>
       </c>
@@ -20475,8 +20482,8 @@
       <c r="BE55" s="9"/>
     </row>
     <row r="56" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A56" s="186"/>
-      <c r="B56" s="217"/>
+      <c r="A56" s="187"/>
+      <c r="B56" s="218"/>
       <c r="C56" s="30" t="s">
         <v>252</v>
       </c>
@@ -20597,7 +20604,7 @@
       <c r="BE57" s="10"/>
     </row>
     <row r="58" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A58" s="184" t="s">
+      <c r="A58" s="185" t="s">
         <v>614</v>
       </c>
       <c r="B58" s="141" t="s">
@@ -20666,7 +20673,7 @@
       <c r="BE58" s="9"/>
     </row>
     <row r="59" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A59" s="185"/>
+      <c r="A59" s="186"/>
       <c r="B59" s="141" t="s">
         <v>43</v>
       </c>
@@ -20733,7 +20740,7 @@
       <c r="BE59" s="9"/>
     </row>
     <row r="60" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A60" s="185"/>
+      <c r="A60" s="186"/>
       <c r="B60" s="141" t="s">
         <v>44</v>
       </c>
@@ -20802,7 +20809,7 @@
       <c r="BE60" s="9"/>
     </row>
     <row r="61" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A61" s="185"/>
+      <c r="A61" s="186"/>
       <c r="B61" s="141" t="s">
         <v>45</v>
       </c>
@@ -20871,8 +20878,8 @@
       <c r="BE61" s="25"/>
     </row>
     <row r="62" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A62" s="185"/>
-      <c r="B62" s="182" t="s">
+      <c r="A62" s="186"/>
+      <c r="B62" s="183" t="s">
         <v>46</v>
       </c>
       <c r="C62" s="31" t="s">
@@ -20942,8 +20949,8 @@
       <c r="BE62" s="9"/>
     </row>
     <row r="63" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A63" s="185"/>
-      <c r="B63" s="183"/>
+      <c r="A63" s="186"/>
+      <c r="B63" s="184"/>
       <c r="C63" s="31" t="s">
         <v>140</v>
       </c>
@@ -21011,7 +21018,7 @@
       <c r="BE63" s="9"/>
     </row>
     <row r="64" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A64" s="185"/>
+      <c r="A64" s="186"/>
       <c r="B64" s="141" t="s">
         <v>47</v>
       </c>
@@ -21088,7 +21095,7 @@
       <c r="BE64" s="18"/>
     </row>
     <row r="65" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A65" s="186"/>
+      <c r="A65" s="187"/>
       <c r="B65" s="142" t="s">
         <v>539</v>
       </c>
@@ -21220,10 +21227,10 @@
       <c r="BE66" s="10"/>
     </row>
     <row r="67" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A67" s="184" t="s">
+      <c r="A67" s="185" t="s">
         <v>605</v>
       </c>
-      <c r="B67" s="241" t="s">
+      <c r="B67" s="242" t="s">
         <v>55</v>
       </c>
       <c r="C67" s="31" t="s">
@@ -21291,8 +21298,8 @@
       <c r="BE67" s="9"/>
     </row>
     <row r="68" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A68" s="185"/>
-      <c r="B68" s="241"/>
+      <c r="A68" s="186"/>
+      <c r="B68" s="242"/>
       <c r="C68" s="31" t="s">
         <v>256</v>
       </c>
@@ -21358,8 +21365,8 @@
       <c r="BE68" s="9"/>
     </row>
     <row r="69" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A69" s="185"/>
-      <c r="B69" s="241" t="s">
+      <c r="A69" s="186"/>
+      <c r="B69" s="242" t="s">
         <v>56</v>
       </c>
       <c r="C69" s="31" t="s">
@@ -21425,8 +21432,8 @@
       <c r="BE69" s="9"/>
     </row>
     <row r="70" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A70" s="185"/>
-      <c r="B70" s="241"/>
+      <c r="A70" s="186"/>
+      <c r="B70" s="242"/>
       <c r="C70" s="31" t="s">
         <v>117</v>
       </c>
@@ -21492,7 +21499,7 @@
       <c r="BE70" s="9"/>
     </row>
     <row r="71" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A71" s="185"/>
+      <c r="A71" s="186"/>
       <c r="B71" s="141" t="s">
         <v>57</v>
       </c>
@@ -21559,7 +21566,7 @@
       <c r="BE71" s="25"/>
     </row>
     <row r="72" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A72" s="185"/>
+      <c r="A72" s="186"/>
       <c r="B72" s="141" t="s">
         <v>58</v>
       </c>
@@ -21626,7 +21633,7 @@
       <c r="BE72" s="25"/>
     </row>
     <row r="73" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A73" s="185"/>
+      <c r="A73" s="186"/>
       <c r="B73" s="141" t="s">
         <v>59</v>
       </c>
@@ -21693,8 +21700,8 @@
       <c r="BE73" s="9"/>
     </row>
     <row r="74" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A74" s="185"/>
-      <c r="B74" s="241" t="s">
+      <c r="A74" s="186"/>
+      <c r="B74" s="242" t="s">
         <v>60</v>
       </c>
       <c r="C74" s="23" t="s">
@@ -21760,8 +21767,8 @@
       <c r="BE74" s="9"/>
     </row>
     <row r="75" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A75" s="185"/>
-      <c r="B75" s="241"/>
+      <c r="A75" s="186"/>
+      <c r="B75" s="242"/>
       <c r="C75" s="23" t="s">
         <v>122</v>
       </c>
@@ -21825,8 +21832,8 @@
       <c r="BE75" s="9"/>
     </row>
     <row r="76" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A76" s="185"/>
-      <c r="B76" s="241"/>
+      <c r="A76" s="186"/>
+      <c r="B76" s="242"/>
       <c r="C76" s="23" t="s">
         <v>123</v>
       </c>
@@ -21890,7 +21897,7 @@
       <c r="BE76" s="9"/>
     </row>
     <row r="77" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A77" s="186"/>
+      <c r="A77" s="187"/>
       <c r="B77" s="143" t="s">
         <v>61</v>
       </c>
@@ -21957,10 +21964,10 @@
       <c r="BE77" s="9"/>
     </row>
     <row r="78" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A78" s="184" t="s">
+      <c r="A78" s="185" t="s">
         <v>615</v>
       </c>
-      <c r="B78" s="182" t="s">
+      <c r="B78" s="183" t="s">
         <v>75</v>
       </c>
       <c r="C78" s="31" t="s">
@@ -22026,8 +22033,8 @@
       <c r="BE78" s="9"/>
     </row>
     <row r="79" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A79" s="185"/>
-      <c r="B79" s="183"/>
+      <c r="A79" s="186"/>
+      <c r="B79" s="184"/>
       <c r="C79" s="31" t="s">
         <v>144</v>
       </c>
@@ -22091,7 +22098,7 @@
       <c r="BE79" s="9"/>
     </row>
     <row r="80" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A80" s="185"/>
+      <c r="A80" s="186"/>
       <c r="B80" s="136" t="s">
         <v>76</v>
       </c>
@@ -22158,8 +22165,8 @@
       <c r="BE80" s="9"/>
     </row>
     <row r="81" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A81" s="185"/>
-      <c r="B81" s="241" t="s">
+      <c r="A81" s="186"/>
+      <c r="B81" s="242" t="s">
         <v>77</v>
       </c>
       <c r="C81" s="23" t="s">
@@ -22225,8 +22232,8 @@
       <c r="BE81" s="9"/>
     </row>
     <row r="82" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A82" s="185"/>
-      <c r="B82" s="241"/>
+      <c r="A82" s="186"/>
+      <c r="B82" s="242"/>
       <c r="C82" s="23" t="s">
         <v>147</v>
       </c>
@@ -22290,7 +22297,7 @@
       <c r="BE82" s="9"/>
     </row>
     <row r="83" spans="1:57" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="185"/>
+      <c r="A83" s="186"/>
       <c r="B83" s="143" t="s">
         <v>78</v>
       </c>
@@ -22359,8 +22366,8 @@
       <c r="BE83" s="25"/>
     </row>
     <row r="84" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A84" s="185"/>
-      <c r="B84" s="182" t="s">
+      <c r="A84" s="186"/>
+      <c r="B84" s="183" t="s">
         <v>79</v>
       </c>
       <c r="C84" s="23" t="s">
@@ -22428,8 +22435,8 @@
       <c r="BE84" s="9"/>
     </row>
     <row r="85" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A85" s="185"/>
-      <c r="B85" s="242"/>
+      <c r="A85" s="186"/>
+      <c r="B85" s="243"/>
       <c r="C85" s="23" t="s">
         <v>560</v>
       </c>
@@ -22495,8 +22502,8 @@
       <c r="BE85" s="9"/>
     </row>
     <row r="86" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A86" s="185"/>
-      <c r="B86" s="183"/>
+      <c r="A86" s="186"/>
+      <c r="B86" s="184"/>
       <c r="C86" s="23" t="s">
         <v>152</v>
       </c>
@@ -22562,7 +22569,7 @@
       <c r="BE86" s="9"/>
     </row>
     <row r="87" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A87" s="185"/>
+      <c r="A87" s="186"/>
       <c r="B87" s="143" t="s">
         <v>80</v>
       </c>
@@ -22633,8 +22640,8 @@
       <c r="BE87" s="9"/>
     </row>
     <row r="88" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A88" s="185"/>
-      <c r="B88" s="182" t="s">
+      <c r="A88" s="186"/>
+      <c r="B88" s="183" t="s">
         <v>81</v>
       </c>
       <c r="C88" s="23" t="s">
@@ -22702,8 +22709,8 @@
       <c r="BE88" s="9"/>
     </row>
     <row r="89" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A89" s="185"/>
-      <c r="B89" s="242"/>
+      <c r="A89" s="186"/>
+      <c r="B89" s="243"/>
       <c r="C89" s="23" t="s">
         <v>151</v>
       </c>
@@ -22769,8 +22776,8 @@
       <c r="BE89" s="9"/>
     </row>
     <row r="90" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A90" s="185"/>
-      <c r="B90" s="242"/>
+      <c r="A90" s="186"/>
+      <c r="B90" s="243"/>
       <c r="C90" s="23" t="s">
         <v>560</v>
       </c>
@@ -22836,8 +22843,8 @@
       <c r="BE90" s="9"/>
     </row>
     <row r="91" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A91" s="186"/>
-      <c r="B91" s="183"/>
+      <c r="A91" s="187"/>
+      <c r="B91" s="184"/>
       <c r="C91" s="23" t="s">
         <v>152</v>
       </c>
@@ -22903,10 +22910,10 @@
       <c r="BE91" s="9"/>
     </row>
     <row r="92" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A92" s="184" t="s">
+      <c r="A92" s="185" t="s">
         <v>616</v>
       </c>
-      <c r="B92" s="182" t="s">
+      <c r="B92" s="183" t="s">
         <v>95</v>
       </c>
       <c r="C92" s="23" t="s">
@@ -22972,8 +22979,8 @@
       <c r="BE92" s="25"/>
     </row>
     <row r="93" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A93" s="186"/>
-      <c r="B93" s="183"/>
+      <c r="A93" s="187"/>
+      <c r="B93" s="184"/>
       <c r="C93" s="23" t="s">
         <v>132</v>
       </c>
@@ -23096,10 +23103,10 @@
       <c r="BE94" s="10"/>
     </row>
     <row r="95" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A95" s="184" t="s">
+      <c r="A95" s="185" t="s">
         <v>112</v>
       </c>
-      <c r="B95" s="241" t="s">
+      <c r="B95" s="242" t="s">
         <v>101</v>
       </c>
       <c r="C95" s="23" t="s">
@@ -23167,8 +23174,8 @@
       <c r="BE95" s="9"/>
     </row>
     <row r="96" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A96" s="185"/>
-      <c r="B96" s="241"/>
+      <c r="A96" s="186"/>
+      <c r="B96" s="242"/>
       <c r="C96" s="23" t="s">
         <v>563</v>
       </c>
@@ -23234,7 +23241,7 @@
       <c r="BE96" s="9"/>
     </row>
     <row r="97" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="186"/>
+      <c r="A97" s="187"/>
       <c r="B97" s="142" t="s">
         <v>561</v>
       </c>
@@ -23300,7 +23307,7 @@
       <c r="BE97" s="9"/>
     </row>
     <row r="98" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A98" s="184" t="s">
+      <c r="A98" s="185" t="s">
         <v>617</v>
       </c>
       <c r="B98" s="143" t="s">
@@ -23369,7 +23376,7 @@
       <c r="BE98" s="9"/>
     </row>
     <row r="99" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A99" s="185"/>
+      <c r="A99" s="186"/>
       <c r="B99" s="142" t="s">
         <v>266</v>
       </c>
@@ -23440,7 +23447,7 @@
       <c r="BE99" s="9"/>
     </row>
     <row r="100" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="186"/>
+      <c r="A100" s="187"/>
       <c r="B100" s="142" t="s">
         <v>265</v>
       </c>
@@ -23506,7 +23513,7 @@
       <c r="BE100" s="9"/>
     </row>
     <row r="101" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="184" t="s">
+      <c r="A101" s="185" t="s">
         <v>618</v>
       </c>
       <c r="B101" s="141" t="s">
@@ -23575,7 +23582,7 @@
       <c r="BE101" s="9"/>
     </row>
     <row r="102" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A102" s="186"/>
+      <c r="A102" s="187"/>
       <c r="B102" s="142" t="s">
         <v>264</v>
       </c>
@@ -23701,7 +23708,7 @@
       <c r="BE103" s="10"/>
     </row>
     <row r="104" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A104" s="184" t="s">
+      <c r="A104" s="185" t="s">
         <v>606</v>
       </c>
       <c r="B104" s="141" t="s">
@@ -23770,7 +23777,7 @@
       <c r="BE104" s="25"/>
     </row>
     <row r="105" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A105" s="185"/>
+      <c r="A105" s="186"/>
       <c r="B105" s="141" t="s">
         <v>540</v>
       </c>
@@ -23837,7 +23844,7 @@
       <c r="BE105" s="25"/>
     </row>
     <row r="106" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A106" s="185"/>
+      <c r="A106" s="186"/>
       <c r="B106" s="141" t="s">
         <v>541</v>
       </c>
@@ -23904,8 +23911,8 @@
       <c r="BE106" s="25"/>
     </row>
     <row r="107" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A107" s="185"/>
-      <c r="B107" s="241" t="s">
+      <c r="A107" s="186"/>
+      <c r="B107" s="242" t="s">
         <v>542</v>
       </c>
       <c r="C107" s="23" t="s">
@@ -23971,8 +23978,8 @@
       <c r="BE107" s="25"/>
     </row>
     <row r="108" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A108" s="185"/>
-      <c r="B108" s="241"/>
+      <c r="A108" s="186"/>
+      <c r="B108" s="242"/>
       <c r="C108" s="23" t="s">
         <v>194</v>
       </c>
@@ -24036,8 +24043,8 @@
       <c r="BE108" s="25"/>
     </row>
     <row r="109" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A109" s="185"/>
-      <c r="B109" s="241"/>
+      <c r="A109" s="186"/>
+      <c r="B109" s="242"/>
       <c r="C109" s="23" t="s">
         <v>195</v>
       </c>
@@ -24101,8 +24108,8 @@
       <c r="BE109" s="25"/>
     </row>
     <row r="110" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A110" s="185"/>
-      <c r="B110" s="241" t="s">
+      <c r="A110" s="186"/>
+      <c r="B110" s="242" t="s">
         <v>543</v>
       </c>
       <c r="C110" s="23" t="s">
@@ -24168,8 +24175,8 @@
       <c r="BE110" s="25"/>
     </row>
     <row r="111" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A111" s="185"/>
-      <c r="B111" s="241"/>
+      <c r="A111" s="186"/>
+      <c r="B111" s="242"/>
       <c r="C111" s="23" t="s">
         <v>548</v>
       </c>
@@ -24233,7 +24240,7 @@
       <c r="BE111" s="25"/>
     </row>
     <row r="112" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A112" s="185"/>
+      <c r="A112" s="186"/>
       <c r="B112" s="141" t="s">
         <v>544</v>
       </c>
@@ -24300,8 +24307,8 @@
       <c r="BE112" s="25"/>
     </row>
     <row r="113" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A113" s="185"/>
-      <c r="B113" s="182" t="s">
+      <c r="A113" s="186"/>
+      <c r="B113" s="183" t="s">
         <v>545</v>
       </c>
       <c r="C113" s="23" t="s">
@@ -24367,8 +24374,8 @@
       <c r="BE113" s="25"/>
     </row>
     <row r="114" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A114" s="185"/>
-      <c r="B114" s="183"/>
+      <c r="A114" s="186"/>
+      <c r="B114" s="184"/>
       <c r="C114" s="23" t="s">
         <v>571</v>
       </c>
@@ -24432,7 +24439,7 @@
       <c r="BE114" s="25"/>
     </row>
     <row r="115" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="A115" s="186"/>
+      <c r="A115" s="187"/>
       <c r="B115" s="141" t="s">
         <v>546</v>
       </c>
@@ -24499,10 +24506,10 @@
       <c r="BE115" s="25"/>
     </row>
     <row r="117" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="B117" s="178" t="s">
+      <c r="B117" s="179" t="s">
         <v>245</v>
       </c>
-      <c r="C117" s="178"/>
+      <c r="C117" s="179"/>
       <c r="D117" s="68" t="s">
         <v>388</v>
       </c>
@@ -24530,19 +24537,19 @@
       <c r="AB117" s="68"/>
     </row>
     <row r="118" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="B118" s="165" t="s">
+      <c r="B118" s="166" t="s">
         <v>346</v>
       </c>
-      <c r="C118" s="165"/>
+      <c r="C118" s="166"/>
       <c r="D118" s="66"/>
       <c r="E118" s="66"/>
       <c r="F118" s="66"/>
     </row>
     <row r="119" spans="1:57" x14ac:dyDescent="0.2">
-      <c r="B119" s="166" t="s">
+      <c r="B119" s="167" t="s">
         <v>347</v>
       </c>
-      <c r="C119" s="166"/>
+      <c r="C119" s="167"/>
       <c r="D119" s="67"/>
       <c r="E119" s="67"/>
       <c r="F119" s="67"/>
@@ -24639,72 +24646,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:56" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="247"/>
-      <c r="C1" s="220" t="s">
+      <c r="B1" s="248"/>
+      <c r="C1" s="221" t="s">
         <v>236</v>
       </c>
-      <c r="D1" s="220"/>
-      <c r="E1" s="220"/>
-      <c r="F1" s="220"/>
-      <c r="G1" s="220"/>
-      <c r="H1" s="220"/>
-      <c r="I1" s="220"/>
-      <c r="J1" s="220"/>
-      <c r="K1" s="220"/>
-      <c r="L1" s="220"/>
-      <c r="M1" s="220"/>
-      <c r="N1" s="220"/>
-      <c r="O1" s="220"/>
+      <c r="D1" s="221"/>
+      <c r="E1" s="221"/>
+      <c r="F1" s="221"/>
+      <c r="G1" s="221"/>
+      <c r="H1" s="221"/>
+      <c r="I1" s="221"/>
+      <c r="J1" s="221"/>
+      <c r="K1" s="221"/>
+      <c r="L1" s="221"/>
+      <c r="M1" s="221"/>
+      <c r="N1" s="221"/>
+      <c r="O1" s="221"/>
       <c r="P1" s="97"/>
-      <c r="Q1" s="220" t="s">
+      <c r="Q1" s="221" t="s">
         <v>241</v>
       </c>
-      <c r="R1" s="220"/>
-      <c r="S1" s="220"/>
+      <c r="R1" s="221"/>
+      <c r="S1" s="221"/>
       <c r="T1" s="97"/>
-      <c r="U1" s="220" t="s">
+      <c r="U1" s="221" t="s">
         <v>237</v>
       </c>
-      <c r="V1" s="220"/>
-      <c r="W1" s="220"/>
-      <c r="X1" s="220"/>
-      <c r="Y1" s="220"/>
-      <c r="Z1" s="220"/>
-      <c r="AA1" s="220"/>
+      <c r="V1" s="221"/>
+      <c r="W1" s="221"/>
+      <c r="X1" s="221"/>
+      <c r="Y1" s="221"/>
+      <c r="Z1" s="221"/>
+      <c r="AA1" s="221"/>
       <c r="AB1" s="97"/>
-      <c r="AC1" s="235" t="s">
+      <c r="AC1" s="236" t="s">
         <v>238</v>
       </c>
-      <c r="AD1" s="236"/>
-      <c r="AE1" s="236"/>
-      <c r="AF1" s="236"/>
-      <c r="AG1" s="236"/>
-      <c r="AH1" s="236"/>
-      <c r="AI1" s="236"/>
-      <c r="AJ1" s="236"/>
-      <c r="AK1" s="236"/>
-      <c r="AL1" s="236"/>
-      <c r="AM1" s="237"/>
+      <c r="AD1" s="237"/>
+      <c r="AE1" s="237"/>
+      <c r="AF1" s="237"/>
+      <c r="AG1" s="237"/>
+      <c r="AH1" s="237"/>
+      <c r="AI1" s="237"/>
+      <c r="AJ1" s="237"/>
+      <c r="AK1" s="237"/>
+      <c r="AL1" s="237"/>
+      <c r="AM1" s="238"/>
       <c r="AN1" s="97"/>
-      <c r="AO1" s="232" t="s">
+      <c r="AO1" s="233" t="s">
         <v>239</v>
       </c>
-      <c r="AP1" s="233"/>
-      <c r="AQ1" s="233"/>
-      <c r="AR1" s="234"/>
+      <c r="AP1" s="234"/>
+      <c r="AQ1" s="234"/>
+      <c r="AR1" s="235"/>
       <c r="AS1" s="97"/>
-      <c r="AT1" s="220" t="s">
+      <c r="AT1" s="221" t="s">
         <v>240</v>
       </c>
-      <c r="AU1" s="220"/>
-      <c r="AV1" s="220"/>
+      <c r="AU1" s="221"/>
+      <c r="AV1" s="221"/>
       <c r="AW1" s="97"/>
-      <c r="AX1" s="229" t="s">
+      <c r="AX1" s="230" t="s">
         <v>246</v>
       </c>
-      <c r="AY1" s="230"/>
-      <c r="AZ1" s="230"/>
-      <c r="BA1" s="231"/>
+      <c r="AY1" s="231"/>
+      <c r="AZ1" s="231"/>
+      <c r="BA1" s="232"/>
       <c r="BB1" s="97"/>
       <c r="BC1" s="98" t="s">
         <v>234</v>
@@ -24714,31 +24721,31 @@
       </c>
     </row>
     <row r="2" spans="1:56" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="247"/>
-      <c r="C2" s="249">
+      <c r="B2" s="248"/>
+      <c r="C2" s="250">
         <v>1</v>
       </c>
-      <c r="D2" s="250"/>
+      <c r="D2" s="251"/>
       <c r="E2" s="41">
         <v>2</v>
       </c>
       <c r="F2" s="41">
         <v>3</v>
       </c>
-      <c r="G2" s="223">
+      <c r="G2" s="224">
         <v>4</v>
       </c>
-      <c r="H2" s="224"/>
+      <c r="H2" s="225"/>
       <c r="I2" s="41">
         <v>5</v>
       </c>
       <c r="J2" s="42">
         <v>6</v>
       </c>
-      <c r="K2" s="214">
+      <c r="K2" s="215">
         <v>7</v>
       </c>
-      <c r="L2" s="215"/>
+      <c r="L2" s="216"/>
       <c r="M2" s="24">
         <v>8</v>
       </c>
@@ -24749,10 +24756,10 @@
         <v>10</v>
       </c>
       <c r="P2" s="36"/>
-      <c r="Q2" s="251">
+      <c r="Q2" s="252">
         <v>1</v>
       </c>
-      <c r="R2" s="222"/>
+      <c r="R2" s="223"/>
       <c r="S2" s="49">
         <v>2</v>
       </c>
@@ -24766,11 +24773,11 @@
       <c r="W2" s="24">
         <v>3</v>
       </c>
-      <c r="X2" s="238">
+      <c r="X2" s="239">
         <v>4</v>
       </c>
-      <c r="Y2" s="239"/>
-      <c r="Z2" s="240"/>
+      <c r="Y2" s="240"/>
+      <c r="Z2" s="241"/>
       <c r="AA2" s="50">
         <v>5</v>
       </c>
@@ -24850,7 +24857,7 @@
       </c>
     </row>
     <row r="3" spans="1:56" s="48" customFormat="1" ht="329" x14ac:dyDescent="0.2">
-      <c r="B3" s="248"/>
+      <c r="B3" s="249"/>
       <c r="C3" s="44" t="s">
         <v>391</v>
       </c>
@@ -24980,11 +24987,11 @@
         <v>630</v>
       </c>
       <c r="AW3" s="45"/>
-      <c r="AX3" s="226" t="s">
+      <c r="AX3" s="227" t="s">
         <v>420</v>
       </c>
-      <c r="AY3" s="227"/>
-      <c r="AZ3" s="228"/>
+      <c r="AY3" s="228"/>
+      <c r="AZ3" s="229"/>
       <c r="BA3" s="46" t="s">
         <v>421</v>
       </c>
@@ -24994,7 +25001,7 @@
       </c>
     </row>
     <row r="4" spans="1:56" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="245" t="s">
+      <c r="A4" s="246" t="s">
         <v>527</v>
       </c>
       <c r="B4" s="119" t="s">
@@ -25055,7 +25062,7 @@
       <c r="BC4" s="11"/>
     </row>
     <row r="5" spans="1:56" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="245"/>
+      <c r="A5" s="246"/>
       <c r="B5" s="119" t="s">
         <v>512</v>
       </c>
@@ -25114,7 +25121,7 @@
       <c r="BC5" s="11"/>
     </row>
     <row r="6" spans="1:56" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="245"/>
+      <c r="A6" s="246"/>
       <c r="B6" s="118" t="s">
         <v>513</v>
       </c>
@@ -25180,7 +25187,7 @@
       <c r="BC6" s="11"/>
     </row>
     <row r="7" spans="1:56" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="245"/>
+      <c r="A7" s="246"/>
       <c r="B7" s="118" t="s">
         <v>514</v>
       </c>
@@ -25245,7 +25252,7 @@
       <c r="BC7" s="11"/>
     </row>
     <row r="8" spans="1:56" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="245"/>
+      <c r="A8" s="246"/>
       <c r="B8" s="118" t="s">
         <v>515</v>
       </c>
@@ -25306,7 +25313,7 @@
       <c r="BC8" s="11"/>
     </row>
     <row r="9" spans="1:56" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="245"/>
+      <c r="A9" s="246"/>
       <c r="B9" s="118" t="s">
         <v>522</v>
       </c>
@@ -25375,7 +25382,7 @@
       <c r="BC9" s="11"/>
     </row>
     <row r="10" spans="1:56" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="245"/>
+      <c r="A10" s="246"/>
       <c r="B10" s="118" t="s">
         <v>523</v>
       </c>
@@ -25442,7 +25449,7 @@
       <c r="BC10" s="11"/>
     </row>
     <row r="11" spans="1:56" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="245"/>
+      <c r="A11" s="246"/>
       <c r="B11" s="118" t="s">
         <v>524</v>
       </c>
@@ -25519,7 +25526,7 @@
       <c r="BC11" s="11"/>
     </row>
     <row r="12" spans="1:56" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="245"/>
+      <c r="A12" s="246"/>
       <c r="B12" s="118" t="s">
         <v>516</v>
       </c>
@@ -25580,7 +25587,7 @@
       <c r="BC12" s="25"/>
     </row>
     <row r="13" spans="1:56" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="245"/>
+      <c r="A13" s="246"/>
       <c r="B13" s="119" t="s">
         <v>517</v>
       </c>
@@ -25639,7 +25646,7 @@
       <c r="BC13" s="25"/>
     </row>
     <row r="14" spans="1:56" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="245"/>
+      <c r="A14" s="246"/>
       <c r="B14" s="119" t="s">
         <v>519</v>
       </c>
@@ -25698,7 +25705,7 @@
       <c r="BC14" s="25"/>
     </row>
     <row r="15" spans="1:56" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="245"/>
+      <c r="A15" s="246"/>
       <c r="B15" s="119" t="s">
         <v>518</v>
       </c>
@@ -25757,7 +25764,7 @@
       <c r="BC15" s="25"/>
     </row>
     <row r="16" spans="1:56" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="245"/>
+      <c r="A16" s="246"/>
       <c r="B16" s="119" t="s">
         <v>520</v>
       </c>
@@ -25816,7 +25823,7 @@
       <c r="BC16" s="25"/>
     </row>
     <row r="17" spans="1:55" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="245"/>
+      <c r="A17" s="246"/>
       <c r="B17" s="119" t="s">
         <v>521</v>
       </c>
@@ -25876,13 +25883,13 @@
     </row>
     <row r="19" spans="1:55" x14ac:dyDescent="0.2">
       <c r="B19" s="3"/>
-      <c r="C19" s="178" t="s">
+      <c r="C19" s="179" t="s">
         <v>245</v>
       </c>
-      <c r="D19" s="178"/>
-      <c r="E19" s="178"/>
-      <c r="F19" s="178"/>
-      <c r="G19" s="178"/>
+      <c r="D19" s="179"/>
+      <c r="E19" s="179"/>
+      <c r="F19" s="179"/>
+      <c r="G19" s="179"/>
       <c r="H19" s="68"/>
       <c r="I19" s="68"/>
       <c r="J19" s="68"/>
@@ -25905,26 +25912,31 @@
     </row>
     <row r="20" spans="1:55" x14ac:dyDescent="0.2">
       <c r="B20" s="3"/>
-      <c r="C20" s="165" t="s">
+      <c r="C20" s="166" t="s">
         <v>525</v>
       </c>
-      <c r="D20" s="165"/>
-      <c r="E20" s="165"/>
-      <c r="F20" s="165"/>
-      <c r="G20" s="165"/>
+      <c r="D20" s="166"/>
+      <c r="E20" s="166"/>
+      <c r="F20" s="166"/>
+      <c r="G20" s="166"/>
     </row>
     <row r="21" spans="1:55" x14ac:dyDescent="0.2">
       <c r="B21" s="3"/>
-      <c r="C21" s="246" t="s">
+      <c r="C21" s="247" t="s">
         <v>526</v>
       </c>
-      <c r="D21" s="246"/>
-      <c r="E21" s="246"/>
-      <c r="F21" s="246"/>
-      <c r="G21" s="246"/>
+      <c r="D21" s="247"/>
+      <c r="E21" s="247"/>
+      <c r="F21" s="247"/>
+      <c r="G21" s="247"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="AO1:AR1"/>
+    <mergeCell ref="A4:A17"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
     <mergeCell ref="C21:G21"/>
     <mergeCell ref="AX3:AZ3"/>
     <mergeCell ref="B1:B3"/>
@@ -25938,11 +25950,6 @@
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="U1:AA1"/>
     <mergeCell ref="AC1:AM1"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="AO1:AR1"/>
-    <mergeCell ref="A4:A17"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="30" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>